<commit_message>
Carla UPDATE LEAVE CARD 3/31/2023 2:51 PM
</commit_message>
<xml_diff>
--- a/ANDAG, ALEX.xlsx
+++ b/ANDAG, ALEX.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\LEAVECARD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DOLE\Desktop\LEAVE-CARD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C1471A7-A9EC-44CE-8F8E-FDE1C0051796}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{2C4B9B69-0AD3-46D4-A495-D1BDE1D16EC6}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="INSTRUCTION" sheetId="4" r:id="rId1"/>
@@ -25,7 +24,7 @@
     <definedName name="BALANCE_1">Table1[[#Headers],[BALANCE]]</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">Sheet1!$1:$9</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="57">
   <si>
     <t>PERIOD</t>
   </si>
@@ -211,7 +210,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
@@ -852,7 +851,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -900,7 +898,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -943,7 +941,7 @@
         <xdr:cNvPr id="5" name="TextBox 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1007,7 +1005,7 @@
         <xdr:cNvPr id="4" name="Arrow: Left 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1067,7 +1065,7 @@
         <xdr:cNvPr id="8" name="Oval 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1133,7 +1131,7 @@
         <xdr:cNvPr id="9" name="Arrow: Left-Right 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1196,7 +1194,7 @@
         <xdr:cNvPr id="10" name="TextBox 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1294,7 +1292,7 @@
         <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1353,7 +1351,7 @@
         <xdr:cNvPr id="19" name="TextBox 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1418,7 +1416,7 @@
         <xdr:cNvPr id="20" name="Picture 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1461,7 +1459,7 @@
         <xdr:cNvPr id="21" name="TextBox 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1536,7 +1534,7 @@
         <xdr:cNvPr id="22" name="TextBox 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1722,7 +1720,7 @@
         <xdr:cNvPr id="23" name="Oval 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1788,7 +1786,7 @@
         <xdr:cNvPr id="24" name="Straight Arrow Connector 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1846,7 +1844,7 @@
         <xdr:cNvPr id="26" name="Oval 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1912,7 +1910,7 @@
         <xdr:cNvPr id="27" name="Straight Arrow Connector 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1968,7 +1966,7 @@
         <xdr:cNvPr id="30" name="TextBox 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2043,7 +2041,7 @@
         <xdr:cNvPr id="31" name="Picture 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2086,7 +2084,7 @@
         <xdr:cNvPr id="32" name="Oval 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2152,7 +2150,7 @@
         <xdr:cNvPr id="33" name="Straight Arrow Connector 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2208,7 +2206,7 @@
         <xdr:cNvPr id="34" name="TextBox 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2304,25 +2302,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D52DCCA-84C7-4E23-9F01-BAD20F9E44D8}" name="Table1" displayName="Table1" ref="A8:K133" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A8:K133" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{29298656-164E-44DD-A190-558D78410746}" name="PERIOD" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{653A013C-2253-41B2-B51E-E0CEE6FCA4B9}" name="PARTICULARS" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{23618FA7-8FE1-47F3-A791-7E4F2612427B}" name="EARNED" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{BA6D2C36-5CF4-40D7-AFDD-218AEBB26721}" name="Absence Undertime W/ Pay" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{44B79BA7-06A4-4888-BFE5-96396FB13C9E}" name="BALANCE" dataDxfId="6">
+    <tableColumn id="1" name="PERIOD" dataDxfId="10"/>
+    <tableColumn id="2" name="PARTICULARS" dataDxfId="9"/>
+    <tableColumn id="3" name="EARNED" dataDxfId="8"/>
+    <tableColumn id="4" name="Absence Undertime W/ Pay" dataDxfId="7"/>
+    <tableColumn id="5" name="BALANCE" dataDxfId="6">
       <calculatedColumnFormula>SUM(Table1[EARNED])-SUM(Table1[Absence Undertime W/ Pay])+CONVERTION!$A$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{1A20B288-1D72-4858-B3C2-871EB9CF011E}" name="Absence Undertime W/O Pay" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{16E84B2D-53AC-4AEA-B1BC-1BC1E2E9B51B}" name="EARNED " dataDxfId="4">
+    <tableColumn id="6" name="Absence Undertime W/O Pay" dataDxfId="5"/>
+    <tableColumn id="7" name="EARNED " dataDxfId="4">
       <calculatedColumnFormula>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{A10DEDBF-F571-4518-A832-0B75654FC984}" name="Absence Undertime  W/ Pay" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{9E225A68-4AC2-420E-B4D1-1378612CB5CD}" name="BALANCE " dataDxfId="2">
+    <tableColumn id="8" name="Absence Undertime  W/ Pay" dataDxfId="3"/>
+    <tableColumn id="9" name="BALANCE " dataDxfId="2">
       <calculatedColumnFormula>SUM(Table1[[EARNED ]])-SUM(Table1[Absence Undertime  W/ Pay])+CONVERTION!$B$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{715FA023-3759-440B-8D8E-42D3E30EC36F}" name="Absence Undertime  W/O Pay" dataDxfId="1"/>
-    <tableColumn id="11" xr3:uid="{7E55BDC4-4FFC-4009-94E5-7F3F3565D56A}" name="REMARKS" dataDxfId="0"/>
+    <tableColumn id="10" name="Absence Undertime  W/O Pay" dataDxfId="1"/>
+    <tableColumn id="11" name="REMARKS" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -2629,7 +2627,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D098C40-D36A-4A12-B6E1-6D049DE49862}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -2639,7 +2637,7 @@
       <selection activeCell="Z62" sqref="Z62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2647,34 +2645,34 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0FF8E2B-FA0C-43AD-94F6-3305AF75672F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:K133"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3576" topLeftCell="A51" activePane="bottomLeft"/>
+      <pane ySplit="3690" topLeftCell="A51" activePane="bottomLeft"/>
       <selection activeCell="F4" sqref="F4:G4"/>
-      <selection pane="bottomLeft" activeCell="B59" sqref="B59"/>
+      <selection pane="bottomLeft" activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="30" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.77734375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" style="30" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.77734375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="24.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="30" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" style="30" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>9</v>
       </c>
@@ -2695,7 +2693,7 @@
       <c r="J2" s="52"/>
       <c r="K2" s="53"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
@@ -2715,7 +2713,7 @@
       <c r="J3" s="54"/>
       <c r="K3" s="55"/>
     </row>
-    <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
@@ -2737,7 +2735,7 @@
       <c r="J4" s="52"/>
       <c r="K4" s="53"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="H5" s="27" t="s">
         <v>18</v>
@@ -2745,7 +2743,7 @@
       <c r="I5" s="27"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
       <c r="B6" s="8"/>
       <c r="C6" s="31"/>
@@ -2758,7 +2756,7 @@
       <c r="J6" s="8"/>
       <c r="K6" s="19"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
       <c r="C7" s="50" t="s">
@@ -2775,7 +2773,7 @@
       <c r="J7" s="50"/>
       <c r="K7" s="14"/>
     </row>
-    <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>0</v>
       </c>
@@ -2810,7 +2808,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="23"/>
       <c r="B9" s="24" t="s">
         <v>23</v>
@@ -2819,7 +2817,7 @@
       <c r="D9" s="11"/>
       <c r="E9" s="13">
         <f>SUM(Table1[EARNED])-SUM(Table1[Absence Undertime W/ Pay])+CONVERTION!$A$3</f>
-        <v>38.75</v>
+        <v>41.25</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="13" t="str">
@@ -2829,12 +2827,12 @@
       <c r="H9" s="11"/>
       <c r="I9" s="13">
         <f>SUM(Table1[[EARNED ]])-SUM(Table1[Absence Undertime  W/ Pay])+CONVERTION!$B$3</f>
-        <v>52.75</v>
+        <v>54.25</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="48" t="s">
         <v>45</v>
       </c>
@@ -2856,7 +2854,7 @@
       <c r="J10" s="11"/>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="40">
         <v>43647</v>
       </c>
@@ -2876,7 +2874,7 @@
       <c r="J11" s="11"/>
       <c r="K11" s="20"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="40">
         <f>EDATE(A11,1)</f>
         <v>43678</v>
@@ -2897,7 +2895,7 @@
       <c r="J12" s="11"/>
       <c r="K12" s="20"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="40">
         <f t="shared" ref="A13:A16" si="0">EDATE(A12,1)</f>
         <v>43709</v>
@@ -2918,7 +2916,7 @@
       <c r="J13" s="11"/>
       <c r="K13" s="20"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="40">
         <f t="shared" si="0"/>
         <v>43739</v>
@@ -2939,7 +2937,7 @@
       <c r="J14" s="11"/>
       <c r="K14" s="20"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="40">
         <f t="shared" si="0"/>
         <v>43770</v>
@@ -2960,7 +2958,7 @@
       <c r="J15" s="11"/>
       <c r="K15" s="20"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="40">
         <f t="shared" si="0"/>
         <v>43800</v>
@@ -2981,7 +2979,7 @@
       <c r="J16" s="12"/>
       <c r="K16" s="15"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="48" t="s">
         <v>46</v>
       </c>
@@ -2999,7 +2997,7 @@
       <c r="J17" s="11"/>
       <c r="K17" s="20"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="40">
         <v>43831</v>
       </c>
@@ -3019,7 +3017,7 @@
       <c r="J18" s="11"/>
       <c r="K18" s="20"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="40">
         <v>43862</v>
       </c>
@@ -3039,7 +3037,7 @@
       <c r="J19" s="11"/>
       <c r="K19" s="20"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="40">
         <v>43891</v>
       </c>
@@ -3059,7 +3057,7 @@
       <c r="J20" s="11"/>
       <c r="K20" s="20"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="40">
         <v>43922</v>
       </c>
@@ -3079,7 +3077,7 @@
       <c r="J21" s="11"/>
       <c r="K21" s="20"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="40">
         <v>43952</v>
       </c>
@@ -3099,7 +3097,7 @@
       <c r="J22" s="11"/>
       <c r="K22" s="20"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="40">
         <v>43983</v>
       </c>
@@ -3119,7 +3117,7 @@
       <c r="J23" s="11"/>
       <c r="K23" s="20"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="40">
         <v>44013</v>
       </c>
@@ -3139,7 +3137,7 @@
       <c r="J24" s="11"/>
       <c r="K24" s="20"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="40">
         <v>44044</v>
       </c>
@@ -3159,7 +3157,7 @@
       <c r="J25" s="11"/>
       <c r="K25" s="20"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="40">
         <v>44075</v>
       </c>
@@ -3179,7 +3177,7 @@
       <c r="J26" s="11"/>
       <c r="K26" s="20"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="40">
         <v>44105</v>
       </c>
@@ -3199,7 +3197,7 @@
       <c r="J27" s="11"/>
       <c r="K27" s="20"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="40">
         <v>44136</v>
       </c>
@@ -3219,7 +3217,7 @@
       <c r="J28" s="11"/>
       <c r="K28" s="20"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="40">
         <v>44166</v>
       </c>
@@ -3243,7 +3241,7 @@
       <c r="J29" s="11"/>
       <c r="K29" s="20"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="48" t="s">
         <v>47</v>
       </c>
@@ -3261,7 +3259,7 @@
       <c r="J30" s="11"/>
       <c r="K30" s="20"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="40">
         <v>44197</v>
       </c>
@@ -3281,7 +3279,7 @@
       <c r="J31" s="11"/>
       <c r="K31" s="20"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="40">
         <v>44228</v>
       </c>
@@ -3301,7 +3299,7 @@
       <c r="J32" s="11"/>
       <c r="K32" s="20"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="40">
         <v>44256</v>
       </c>
@@ -3321,7 +3319,7 @@
       <c r="J33" s="11"/>
       <c r="K33" s="20"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="40">
         <v>44287</v>
       </c>
@@ -3341,7 +3339,7 @@
       <c r="J34" s="11"/>
       <c r="K34" s="20"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="40">
         <v>44317</v>
       </c>
@@ -3361,7 +3359,7 @@
       <c r="J35" s="11"/>
       <c r="K35" s="20"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="40">
         <v>44348</v>
       </c>
@@ -3381,7 +3379,7 @@
       <c r="J36" s="11"/>
       <c r="K36" s="20"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="40">
         <v>44378</v>
       </c>
@@ -3401,7 +3399,7 @@
       <c r="J37" s="11"/>
       <c r="K37" s="20"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="40">
         <v>44409</v>
       </c>
@@ -3421,7 +3419,7 @@
       <c r="J38" s="11"/>
       <c r="K38" s="20"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="40">
         <v>44440</v>
       </c>
@@ -3441,7 +3439,7 @@
       <c r="J39" s="11"/>
       <c r="K39" s="20"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="40">
         <v>44470</v>
       </c>
@@ -3461,7 +3459,7 @@
       <c r="J40" s="11"/>
       <c r="K40" s="20"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="40">
         <v>44501</v>
       </c>
@@ -3481,7 +3479,7 @@
       <c r="J41" s="11"/>
       <c r="K41" s="20"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="40">
         <v>44531</v>
       </c>
@@ -3505,7 +3503,7 @@
       <c r="J42" s="11"/>
       <c r="K42" s="20"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="48" t="s">
         <v>49</v>
       </c>
@@ -3523,7 +3521,7 @@
       <c r="J43" s="11"/>
       <c r="K43" s="20"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="40">
         <v>44562</v>
       </c>
@@ -3543,7 +3541,7 @@
       <c r="J44" s="11"/>
       <c r="K44" s="20"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="40">
         <v>44593</v>
       </c>
@@ -3563,7 +3561,7 @@
       <c r="J45" s="11"/>
       <c r="K45" s="20"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="40">
         <v>44621</v>
       </c>
@@ -3583,7 +3581,7 @@
       <c r="J46" s="11"/>
       <c r="K46" s="20"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="40">
         <v>44652</v>
       </c>
@@ -3603,7 +3601,7 @@
       <c r="J47" s="11"/>
       <c r="K47" s="20"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="40">
         <v>44682</v>
       </c>
@@ -3629,7 +3627,7 @@
         <v>44687</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="40">
         <v>44713</v>
       </c>
@@ -3649,7 +3647,7 @@
       <c r="J49" s="11"/>
       <c r="K49" s="20"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="40">
         <v>44743</v>
       </c>
@@ -3669,7 +3667,7 @@
       <c r="J50" s="11"/>
       <c r="K50" s="20"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="40">
         <v>44774</v>
       </c>
@@ -3689,7 +3687,7 @@
       <c r="J51" s="11"/>
       <c r="K51" s="20"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="40">
         <v>44805</v>
       </c>
@@ -3709,7 +3707,7 @@
       <c r="J52" s="11"/>
       <c r="K52" s="20"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="40">
         <v>44835</v>
       </c>
@@ -3729,7 +3727,7 @@
       <c r="J53" s="11"/>
       <c r="K53" s="20"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="40">
         <v>44866</v>
       </c>
@@ -3755,7 +3753,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="40"/>
       <c r="B55" s="20" t="s">
         <v>54</v>
@@ -3777,7 +3775,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="40"/>
       <c r="B56" s="20" t="s">
         <v>56</v>
@@ -3797,7 +3795,7 @@
         <v>44893</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="40">
         <v>44896</v>
       </c>
@@ -3817,7 +3815,7 @@
       <c r="J57" s="11"/>
       <c r="K57" s="20"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="48" t="s">
         <v>53</v>
       </c>
@@ -3835,7 +3833,7 @@
       <c r="J58" s="11"/>
       <c r="K58" s="20"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="40">
         <v>44927</v>
       </c>
@@ -3855,43 +3853,53 @@
       <c r="J59" s="11"/>
       <c r="K59" s="20"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="40">
         <v>44958</v>
       </c>
-      <c r="B60" s="20"/>
-      <c r="C60" s="13"/>
+      <c r="B60" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C60" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D60" s="39"/>
       <c r="E60" s="9"/>
       <c r="F60" s="20"/>
-      <c r="G60" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
-      </c>
-      <c r="H60" s="39"/>
+      <c r="G60" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
+      </c>
+      <c r="H60" s="39">
+        <v>1</v>
+      </c>
       <c r="I60" s="9"/>
       <c r="J60" s="11"/>
-      <c r="K60" s="20"/>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K60" s="49">
+        <v>44962</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="40">
         <v>44986</v>
       </c>
       <c r="B61" s="20"/>
-      <c r="C61" s="13"/>
+      <c r="C61" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D61" s="39"/>
       <c r="E61" s="9"/>
       <c r="F61" s="20"/>
-      <c r="G61" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G61" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H61" s="39"/>
       <c r="I61" s="9"/>
       <c r="J61" s="11"/>
       <c r="K61" s="20"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="40">
         <v>45017</v>
       </c>
@@ -3909,7 +3917,7 @@
       <c r="J62" s="11"/>
       <c r="K62" s="20"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="40">
         <v>45047</v>
       </c>
@@ -3927,7 +3935,7 @@
       <c r="J63" s="11"/>
       <c r="K63" s="20"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="40">
         <v>45078</v>
       </c>
@@ -3945,7 +3953,7 @@
       <c r="J64" s="11"/>
       <c r="K64" s="20"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="40">
         <v>45108</v>
       </c>
@@ -3963,7 +3971,7 @@
       <c r="J65" s="11"/>
       <c r="K65" s="20"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="40">
         <v>45139</v>
       </c>
@@ -3981,7 +3989,7 @@
       <c r="J66" s="11"/>
       <c r="K66" s="20"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="40">
         <v>45170</v>
       </c>
@@ -3999,7 +4007,7 @@
       <c r="J67" s="11"/>
       <c r="K67" s="20"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="40">
         <v>45200</v>
       </c>
@@ -4017,7 +4025,7 @@
       <c r="J68" s="11"/>
       <c r="K68" s="20"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="40">
         <v>45231</v>
       </c>
@@ -4035,7 +4043,7 @@
       <c r="J69" s="11"/>
       <c r="K69" s="20"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="40">
         <v>45261</v>
       </c>
@@ -4053,7 +4061,7 @@
       <c r="J70" s="11"/>
       <c r="K70" s="20"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="40">
         <v>45292</v>
       </c>
@@ -4071,7 +4079,7 @@
       <c r="J71" s="11"/>
       <c r="K71" s="20"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="40">
         <v>45323</v>
       </c>
@@ -4089,7 +4097,7 @@
       <c r="J72" s="11"/>
       <c r="K72" s="20"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="40">
         <v>45352</v>
       </c>
@@ -4107,7 +4115,7 @@
       <c r="J73" s="11"/>
       <c r="K73" s="20"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="40">
         <v>45383</v>
       </c>
@@ -4125,7 +4133,7 @@
       <c r="J74" s="11"/>
       <c r="K74" s="20"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="40">
         <v>45413</v>
       </c>
@@ -4143,7 +4151,7 @@
       <c r="J75" s="11"/>
       <c r="K75" s="20"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="40">
         <v>45444</v>
       </c>
@@ -4161,7 +4169,7 @@
       <c r="J76" s="11"/>
       <c r="K76" s="20"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="40">
         <v>45474</v>
       </c>
@@ -4179,7 +4187,7 @@
       <c r="J77" s="11"/>
       <c r="K77" s="20"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="40">
         <v>45505</v>
       </c>
@@ -4197,7 +4205,7 @@
       <c r="J78" s="11"/>
       <c r="K78" s="20"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="40">
         <v>45536</v>
       </c>
@@ -4215,7 +4223,7 @@
       <c r="J79" s="11"/>
       <c r="K79" s="20"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="40">
         <v>45566</v>
       </c>
@@ -4233,7 +4241,7 @@
       <c r="J80" s="11"/>
       <c r="K80" s="20"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="40">
         <v>45597</v>
       </c>
@@ -4251,7 +4259,7 @@
       <c r="J81" s="11"/>
       <c r="K81" s="20"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="40">
         <v>45627</v>
       </c>
@@ -4269,7 +4277,7 @@
       <c r="J82" s="11"/>
       <c r="K82" s="20"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="40">
         <v>45658</v>
       </c>
@@ -4287,7 +4295,7 @@
       <c r="J83" s="11"/>
       <c r="K83" s="20"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="40">
         <v>45689</v>
       </c>
@@ -4305,7 +4313,7 @@
       <c r="J84" s="11"/>
       <c r="K84" s="20"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="40">
         <v>45717</v>
       </c>
@@ -4323,7 +4331,7 @@
       <c r="J85" s="11"/>
       <c r="K85" s="20"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="40">
         <v>45748</v>
       </c>
@@ -4341,7 +4349,7 @@
       <c r="J86" s="11"/>
       <c r="K86" s="20"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="40">
         <v>45778</v>
       </c>
@@ -4359,7 +4367,7 @@
       <c r="J87" s="11"/>
       <c r="K87" s="20"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="40">
         <v>45809</v>
       </c>
@@ -4377,7 +4385,7 @@
       <c r="J88" s="11"/>
       <c r="K88" s="20"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="40">
         <v>45839</v>
       </c>
@@ -4395,7 +4403,7 @@
       <c r="J89" s="11"/>
       <c r="K89" s="20"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="40">
         <v>45870</v>
       </c>
@@ -4413,7 +4421,7 @@
       <c r="J90" s="11"/>
       <c r="K90" s="20"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="40">
         <v>45901</v>
       </c>
@@ -4431,7 +4439,7 @@
       <c r="J91" s="11"/>
       <c r="K91" s="20"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="40">
         <v>45931</v>
       </c>
@@ -4449,7 +4457,7 @@
       <c r="J92" s="11"/>
       <c r="K92" s="20"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="40">
         <v>45962</v>
       </c>
@@ -4467,7 +4475,7 @@
       <c r="J93" s="11"/>
       <c r="K93" s="20"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="40">
         <v>45992</v>
       </c>
@@ -4485,7 +4493,7 @@
       <c r="J94" s="11"/>
       <c r="K94" s="20"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="40">
         <v>46023</v>
       </c>
@@ -4503,7 +4511,7 @@
       <c r="J95" s="11"/>
       <c r="K95" s="20"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="40">
         <v>46054</v>
       </c>
@@ -4521,7 +4529,7 @@
       <c r="J96" s="11"/>
       <c r="K96" s="20"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="40">
         <v>46082</v>
       </c>
@@ -4539,7 +4547,7 @@
       <c r="J97" s="11"/>
       <c r="K97" s="20"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="40">
         <v>46113</v>
       </c>
@@ -4557,7 +4565,7 @@
       <c r="J98" s="11"/>
       <c r="K98" s="20"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="40">
         <v>46143</v>
       </c>
@@ -4575,7 +4583,7 @@
       <c r="J99" s="11"/>
       <c r="K99" s="20"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="40">
         <v>46174</v>
       </c>
@@ -4593,7 +4601,7 @@
       <c r="J100" s="11"/>
       <c r="K100" s="20"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="40">
         <v>46204</v>
       </c>
@@ -4611,7 +4619,7 @@
       <c r="J101" s="11"/>
       <c r="K101" s="20"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="40">
         <v>46235</v>
       </c>
@@ -4629,7 +4637,7 @@
       <c r="J102" s="11"/>
       <c r="K102" s="20"/>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="40">
         <v>46266</v>
       </c>
@@ -4647,7 +4655,7 @@
       <c r="J103" s="11"/>
       <c r="K103" s="20"/>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="40">
         <v>46296</v>
       </c>
@@ -4665,7 +4673,7 @@
       <c r="J104" s="11"/>
       <c r="K104" s="20"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="40">
         <v>46327</v>
       </c>
@@ -4683,7 +4691,7 @@
       <c r="J105" s="11"/>
       <c r="K105" s="20"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="40">
         <v>46357</v>
       </c>
@@ -4701,7 +4709,7 @@
       <c r="J106" s="11"/>
       <c r="K106" s="20"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="40">
         <v>46388</v>
       </c>
@@ -4719,7 +4727,7 @@
       <c r="J107" s="11"/>
       <c r="K107" s="20"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="40">
         <v>46419</v>
       </c>
@@ -4737,7 +4745,7 @@
       <c r="J108" s="11"/>
       <c r="K108" s="20"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="40">
         <v>46447</v>
       </c>
@@ -4755,7 +4763,7 @@
       <c r="J109" s="11"/>
       <c r="K109" s="20"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="40">
         <v>46478</v>
       </c>
@@ -4773,7 +4781,7 @@
       <c r="J110" s="11"/>
       <c r="K110" s="20"/>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="40">
         <v>46508</v>
       </c>
@@ -4791,7 +4799,7 @@
       <c r="J111" s="11"/>
       <c r="K111" s="20"/>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="40"/>
       <c r="B112" s="20"/>
       <c r="C112" s="13"/>
@@ -4807,7 +4815,7 @@
       <c r="J112" s="11"/>
       <c r="K112" s="20"/>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="40"/>
       <c r="B113" s="20"/>
       <c r="C113" s="13"/>
@@ -4823,7 +4831,7 @@
       <c r="J113" s="11"/>
       <c r="K113" s="20"/>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="40"/>
       <c r="B114" s="20"/>
       <c r="C114" s="13"/>
@@ -4839,7 +4847,7 @@
       <c r="J114" s="11"/>
       <c r="K114" s="20"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="40"/>
       <c r="B115" s="20"/>
       <c r="C115" s="13"/>
@@ -4855,7 +4863,7 @@
       <c r="J115" s="11"/>
       <c r="K115" s="20"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="40"/>
       <c r="B116" s="20"/>
       <c r="C116" s="13"/>
@@ -4871,7 +4879,7 @@
       <c r="J116" s="11"/>
       <c r="K116" s="20"/>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="40"/>
       <c r="B117" s="20"/>
       <c r="C117" s="13"/>
@@ -4887,7 +4895,7 @@
       <c r="J117" s="11"/>
       <c r="K117" s="20"/>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="40"/>
       <c r="B118" s="20"/>
       <c r="C118" s="13"/>
@@ -4903,7 +4911,7 @@
       <c r="J118" s="11"/>
       <c r="K118" s="20"/>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="40"/>
       <c r="B119" s="20"/>
       <c r="C119" s="13"/>
@@ -4919,7 +4927,7 @@
       <c r="J119" s="11"/>
       <c r="K119" s="20"/>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="40"/>
       <c r="B120" s="20"/>
       <c r="C120" s="13"/>
@@ -4935,7 +4943,7 @@
       <c r="J120" s="11"/>
       <c r="K120" s="20"/>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" s="40"/>
       <c r="B121" s="20"/>
       <c r="C121" s="13"/>
@@ -4951,7 +4959,7 @@
       <c r="J121" s="11"/>
       <c r="K121" s="20"/>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="40"/>
       <c r="B122" s="20"/>
       <c r="C122" s="13"/>
@@ -4967,7 +4975,7 @@
       <c r="J122" s="11"/>
       <c r="K122" s="20"/>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="40"/>
       <c r="B123" s="20"/>
       <c r="C123" s="13"/>
@@ -4983,7 +4991,7 @@
       <c r="J123" s="11"/>
       <c r="K123" s="20"/>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="40"/>
       <c r="B124" s="20"/>
       <c r="C124" s="13"/>
@@ -4999,7 +5007,7 @@
       <c r="J124" s="11"/>
       <c r="K124" s="20"/>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" s="40"/>
       <c r="B125" s="20"/>
       <c r="C125" s="13"/>
@@ -5015,7 +5023,7 @@
       <c r="J125" s="11"/>
       <c r="K125" s="20"/>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" s="40"/>
       <c r="B126" s="20"/>
       <c r="C126" s="13"/>
@@ -5031,7 +5039,7 @@
       <c r="J126" s="11"/>
       <c r="K126" s="20"/>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" s="40"/>
       <c r="B127" s="20"/>
       <c r="C127" s="13"/>
@@ -5047,7 +5055,7 @@
       <c r="J127" s="11"/>
       <c r="K127" s="20"/>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" s="40"/>
       <c r="B128" s="20"/>
       <c r="C128" s="13"/>
@@ -5063,7 +5071,7 @@
       <c r="J128" s="11"/>
       <c r="K128" s="20"/>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" s="40"/>
       <c r="B129" s="20"/>
       <c r="C129" s="13"/>
@@ -5079,7 +5087,7 @@
       <c r="J129" s="11"/>
       <c r="K129" s="20"/>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" s="40"/>
       <c r="B130" s="20"/>
       <c r="C130" s="13"/>
@@ -5095,7 +5103,7 @@
       <c r="J130" s="11"/>
       <c r="K130" s="20"/>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" s="40"/>
       <c r="B131" s="20"/>
       <c r="C131" s="13"/>
@@ -5111,7 +5119,7 @@
       <c r="J131" s="11"/>
       <c r="K131" s="20"/>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="40"/>
       <c r="B132" s="20"/>
       <c r="C132" s="13"/>
@@ -5127,7 +5135,7 @@
       <c r="J132" s="11"/>
       <c r="K132" s="20"/>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" s="41"/>
       <c r="B133" s="15"/>
       <c r="C133" s="42"/>
@@ -5158,10 +5166,10 @@
     <mergeCell ref="F4:G4"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2" xr:uid="{3C67B38A-DE91-4BA1-85D0-F5C61D6395E6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2">
       <formula1>"1 - Married (and not separated), 2 - Widowed (including living common law), 3 - Separated (including living common law), 4 - Divorced (including living common law), 5 - Single (including living common law)"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4" xr:uid="{C9F25C0C-606E-415B-87B4-B098DE141EB5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4">
       <formula1>"PERMANENT, CO-TERMINUS, CASUAL, JOBCON"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5184,28 +5192,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CB8F789-193C-43F9-8D48-B0DEE5C76ADA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I1" sqref="I1:L1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.21875" customWidth="1"/>
-    <col min="2" max="2" width="20.77734375" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.109375" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" customWidth="1"/>
-    <col min="11" max="11" width="14.88671875" style="37" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.140625" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" style="37" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D1" s="58" t="s">
         <v>33</v>
       </c>
@@ -5218,7 +5226,7 @@
       <c r="K1" s="59"/>
       <c r="L1" s="59"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>24</v>
       </c>
@@ -5247,7 +5255,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="D3" s="11"/>
@@ -5267,17 +5275,17 @@
         <v>---</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="G4" s="33"/>
       <c r="J4" s="1" t="str">
         <f>IF(TEXT(J3,"D")=1,1,TEXT(J3,"D"))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C6" s="38" t="s">
         <v>28</v>
       </c>
@@ -5298,7 +5306,7 @@
       <c r="K6" s="60"/>
       <c r="L6" s="60"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C7" s="37">
         <v>1</v>
       </c>
@@ -5325,7 +5333,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C8" s="37">
         <v>2</v>
       </c>
@@ -5351,7 +5359,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C9" s="37">
         <v>3</v>
       </c>
@@ -5377,7 +5385,7 @@
         <v>8.3000000000000004E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C10" s="37">
         <v>4</v>
       </c>
@@ -5403,7 +5411,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C11" s="37">
         <v>5</v>
       </c>
@@ -5429,7 +5437,7 @@
         <v>0.16700000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C12" s="37">
         <v>6</v>
       </c>
@@ -5455,7 +5463,7 @@
         <v>0.20800000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C13" s="37">
         <v>7</v>
       </c>
@@ -5481,7 +5489,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C14" s="37">
         <v>8</v>
       </c>
@@ -5507,7 +5515,7 @@
         <v>0.29199999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C15" s="37">
         <v>9</v>
       </c>
@@ -5527,7 +5535,7 @@
         <v>0.33299999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C16" s="37">
         <v>10</v>
       </c>
@@ -5547,7 +5555,7 @@
         <v>0.37499999999999994</v>
       </c>
     </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C17" s="37">
         <v>11</v>
       </c>
@@ -5567,7 +5575,7 @@
         <v>0.41699999999999993</v>
       </c>
     </row>
-    <row r="18" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C18" s="37">
         <v>12</v>
       </c>
@@ -5588,7 +5596,7 @@
         <v>0.45799999999999991</v>
       </c>
     </row>
-    <row r="19" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C19" s="37">
         <v>13</v>
       </c>
@@ -5609,7 +5617,7 @@
         <v>0.49999999999999989</v>
       </c>
     </row>
-    <row r="20" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C20" s="37">
         <v>14</v>
       </c>
@@ -5630,7 +5638,7 @@
         <v>0.54199999999999993</v>
       </c>
     </row>
-    <row r="21" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C21" s="37">
         <v>15</v>
       </c>
@@ -5651,7 +5659,7 @@
         <v>0.58299999999999996</v>
       </c>
     </row>
-    <row r="22" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C22" s="37">
         <v>16</v>
       </c>
@@ -5672,7 +5680,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="23" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C23" s="37">
         <v>17</v>
       </c>
@@ -5693,7 +5701,7 @@
         <v>0.66700000000000004</v>
       </c>
     </row>
-    <row r="24" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C24" s="37">
         <v>18</v>
       </c>
@@ -5714,7 +5722,7 @@
         <v>0.70800000000000007</v>
       </c>
     </row>
-    <row r="25" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C25" s="37">
         <v>19</v>
       </c>
@@ -5735,7 +5743,7 @@
         <v>0.75000000000000011</v>
       </c>
     </row>
-    <row r="26" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C26" s="37">
         <v>20</v>
       </c>
@@ -5756,7 +5764,7 @@
         <v>0.79200000000000015</v>
       </c>
     </row>
-    <row r="27" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C27" s="37">
         <v>21</v>
       </c>
@@ -5777,7 +5785,7 @@
         <v>0.83300000000000018</v>
       </c>
     </row>
-    <row r="28" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C28" s="37">
         <v>22</v>
       </c>
@@ -5798,7 +5806,7 @@
         <v>0.87500000000000022</v>
       </c>
     </row>
-    <row r="29" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C29" s="37">
         <v>23</v>
       </c>
@@ -5819,7 +5827,7 @@
         <v>0.91700000000000026</v>
       </c>
     </row>
-    <row r="30" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C30" s="37">
         <v>24</v>
       </c>
@@ -5840,7 +5848,7 @@
         <v>0.9580000000000003</v>
       </c>
     </row>
-    <row r="31" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C31" s="37">
         <v>25</v>
       </c>
@@ -5861,7 +5869,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="32" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C32" s="37">
         <v>26</v>
       </c>
@@ -5882,7 +5890,7 @@
         <v>1.0420000000000003</v>
       </c>
     </row>
-    <row r="33" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C33" s="37">
         <v>27</v>
       </c>
@@ -5903,7 +5911,7 @@
         <v>1.0830000000000002</v>
       </c>
     </row>
-    <row r="34" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C34" s="37">
         <v>28</v>
       </c>
@@ -5924,7 +5932,7 @@
         <v>1.1250000000000002</v>
       </c>
     </row>
-    <row r="35" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C35" s="37">
         <v>29</v>
       </c>
@@ -5945,7 +5953,7 @@
         <v>1.1670000000000003</v>
       </c>
     </row>
-    <row r="36" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C36" s="37">
         <v>30</v>
       </c>
@@ -5966,7 +5974,7 @@
         <v>1.2080000000000002</v>
       </c>
     </row>
-    <row r="37" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C37" s="37">
         <v>31</v>
       </c>
@@ -5987,7 +5995,7 @@
         <v>1.2500000000000002</v>
       </c>
     </row>
-    <row r="38" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C38" s="37">
         <v>32</v>
       </c>
@@ -5996,7 +6004,7 @@
       </c>
       <c r="G38"/>
     </row>
-    <row r="39" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C39" s="37">
         <v>33</v>
       </c>
@@ -6005,7 +6013,7 @@
       </c>
       <c r="G39"/>
     </row>
-    <row r="40" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C40" s="37">
         <v>34</v>
       </c>
@@ -6014,7 +6022,7 @@
       </c>
       <c r="G40"/>
     </row>
-    <row r="41" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C41" s="37">
         <v>35</v>
       </c>
@@ -6023,7 +6031,7 @@
       </c>
       <c r="G41"/>
     </row>
-    <row r="42" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C42" s="37">
         <v>36</v>
       </c>
@@ -6032,7 +6040,7 @@
       </c>
       <c r="G42"/>
     </row>
-    <row r="43" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C43" s="37">
         <v>37</v>
       </c>
@@ -6041,7 +6049,7 @@
       </c>
       <c r="G43"/>
     </row>
-    <row r="44" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C44" s="37">
         <v>38</v>
       </c>
@@ -6050,7 +6058,7 @@
       </c>
       <c r="G44"/>
     </row>
-    <row r="45" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C45" s="37">
         <v>39</v>
       </c>
@@ -6059,7 +6067,7 @@
       </c>
       <c r="G45"/>
     </row>
-    <row r="46" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C46" s="37">
         <v>40</v>
       </c>
@@ -6068,7 +6076,7 @@
       </c>
       <c r="G46"/>
     </row>
-    <row r="47" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C47" s="37">
         <v>41</v>
       </c>
@@ -6077,7 +6085,7 @@
       </c>
       <c r="G47"/>
     </row>
-    <row r="48" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C48" s="37">
         <v>42</v>
       </c>
@@ -6086,7 +6094,7 @@
       </c>
       <c r="G48"/>
     </row>
-    <row r="49" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C49" s="37">
         <v>43</v>
       </c>
@@ -6095,7 +6103,7 @@
       </c>
       <c r="G49"/>
     </row>
-    <row r="50" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C50" s="37">
         <v>44</v>
       </c>
@@ -6104,7 +6112,7 @@
       </c>
       <c r="G50"/>
     </row>
-    <row r="51" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C51" s="37">
         <v>45</v>
       </c>
@@ -6113,7 +6121,7 @@
       </c>
       <c r="G51"/>
     </row>
-    <row r="52" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C52" s="37">
         <v>46</v>
       </c>
@@ -6122,7 +6130,7 @@
       </c>
       <c r="G52"/>
     </row>
-    <row r="53" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C53" s="37">
         <v>47</v>
       </c>
@@ -6131,7 +6139,7 @@
       </c>
       <c r="G53"/>
     </row>
-    <row r="54" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C54" s="37">
         <v>48</v>
       </c>
@@ -6140,7 +6148,7 @@
       </c>
       <c r="G54"/>
     </row>
-    <row r="55" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C55" s="37">
         <v>49</v>
       </c>
@@ -6149,7 +6157,7 @@
       </c>
       <c r="G55"/>
     </row>
-    <row r="56" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C56" s="37">
         <v>50</v>
       </c>
@@ -6158,7 +6166,7 @@
       </c>
       <c r="G56"/>
     </row>
-    <row r="57" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C57" s="37">
         <v>51</v>
       </c>
@@ -6167,7 +6175,7 @@
       </c>
       <c r="G57"/>
     </row>
-    <row r="58" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C58" s="37">
         <v>52</v>
       </c>
@@ -6176,7 +6184,7 @@
       </c>
       <c r="G58"/>
     </row>
-    <row r="59" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C59" s="37">
         <v>53</v>
       </c>
@@ -6185,7 +6193,7 @@
       </c>
       <c r="G59"/>
     </row>
-    <row r="60" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C60" s="37">
         <v>54</v>
       </c>
@@ -6194,7 +6202,7 @@
       </c>
       <c r="G60"/>
     </row>
-    <row r="61" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C61" s="37">
         <v>55</v>
       </c>
@@ -6203,7 +6211,7 @@
       </c>
       <c r="G61"/>
     </row>
-    <row r="62" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C62" s="37">
         <v>56</v>
       </c>
@@ -6212,7 +6220,7 @@
       </c>
       <c r="G62"/>
     </row>
-    <row r="63" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C63" s="37">
         <v>57</v>
       </c>
@@ -6221,7 +6229,7 @@
       </c>
       <c r="G63"/>
     </row>
-    <row r="64" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C64" s="37">
         <v>58</v>
       </c>
@@ -6230,7 +6238,7 @@
       </c>
       <c r="G64"/>
     </row>
-    <row r="65" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C65" s="37">
         <v>59</v>
       </c>
@@ -6239,7 +6247,7 @@
       </c>
       <c r="G65"/>
     </row>
-    <row r="66" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C66" s="37">
         <v>60</v>
       </c>
@@ -6248,7 +6256,7 @@
       </c>
       <c r="G66"/>
     </row>
-    <row r="67" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="3:12" x14ac:dyDescent="0.25">
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>

</xml_diff>

<commit_message>
Update Leave Card 4/27/2023 4:55 PM
</commit_message>
<xml_diff>
--- a/ANDAG, ALEX.xlsx
+++ b/ANDAG, ALEX.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DOLE\Desktop\LEAVE-CARD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\DESKTOP-JHL336T\Users\ASUS\Desktop\LEAVE-CARD\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="57">
   <si>
     <t>PERIOD</t>
   </si>
@@ -898,7 +898,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -941,7 +941,7 @@
         <xdr:cNvPr id="5" name="TextBox 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1005,7 +1005,7 @@
         <xdr:cNvPr id="4" name="Arrow: Left 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1065,7 +1065,7 @@
         <xdr:cNvPr id="8" name="Oval 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1131,7 +1131,7 @@
         <xdr:cNvPr id="9" name="Arrow: Left-Right 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1194,7 +1194,7 @@
         <xdr:cNvPr id="10" name="TextBox 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1292,7 +1292,7 @@
         <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1351,7 +1351,7 @@
         <xdr:cNvPr id="19" name="TextBox 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1416,7 +1416,7 @@
         <xdr:cNvPr id="20" name="Picture 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1459,7 +1459,7 @@
         <xdr:cNvPr id="21" name="TextBox 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1534,7 +1534,7 @@
         <xdr:cNvPr id="22" name="TextBox 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1720,7 +1720,7 @@
         <xdr:cNvPr id="23" name="Oval 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1786,7 +1786,7 @@
         <xdr:cNvPr id="24" name="Straight Arrow Connector 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1844,7 +1844,7 @@
         <xdr:cNvPr id="26" name="Oval 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1910,7 +1910,7 @@
         <xdr:cNvPr id="27" name="Straight Arrow Connector 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1966,7 +1966,7 @@
         <xdr:cNvPr id="30" name="TextBox 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2041,7 +2041,7 @@
         <xdr:cNvPr id="31" name="Picture 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2084,7 +2084,7 @@
         <xdr:cNvPr id="32" name="Oval 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2150,7 +2150,7 @@
         <xdr:cNvPr id="33" name="Straight Arrow Connector 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2206,7 +2206,7 @@
         <xdr:cNvPr id="34" name="TextBox 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2652,9 +2652,9 @@
   <dimension ref="A2:K133"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3690" topLeftCell="A51" activePane="bottomLeft"/>
+      <pane ySplit="3690" topLeftCell="A55" activePane="bottomLeft"/>
       <selection activeCell="F4" sqref="F4:G4"/>
-      <selection pane="bottomLeft" activeCell="B61" sqref="B61"/>
+      <selection pane="bottomLeft" activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2827,7 +2827,7 @@
       <c r="H9" s="11"/>
       <c r="I9" s="13">
         <f>SUM(Table1[[EARNED ]])-SUM(Table1[Absence Undertime  W/ Pay])+CONVERTION!$B$3</f>
-        <v>54.25</v>
+        <v>53.25</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
@@ -3903,7 +3903,9 @@
       <c r="A62" s="40">
         <v>45017</v>
       </c>
-      <c r="B62" s="20"/>
+      <c r="B62" s="20" t="s">
+        <v>50</v>
+      </c>
       <c r="C62" s="13"/>
       <c r="D62" s="39"/>
       <c r="E62" s="9"/>
@@ -3912,10 +3914,14 @@
         <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
         <v/>
       </c>
-      <c r="H62" s="39"/>
+      <c r="H62" s="39">
+        <v>1</v>
+      </c>
       <c r="I62" s="9"/>
       <c r="J62" s="11"/>
-      <c r="K62" s="20"/>
+      <c r="K62" s="49">
+        <v>45037</v>
+      </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="40">

</xml_diff>

<commit_message>
Update Leave Card 5/10/2023 11:17 AM
</commit_message>
<xml_diff>
--- a/ANDAG, ALEX.xlsx
+++ b/ANDAG, ALEX.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="59">
   <si>
     <t>PERIOD</t>
   </si>
@@ -205,6 +205,12 @@
   </si>
   <si>
     <t>SP(1-0-0)</t>
+  </si>
+  <si>
+    <t>5/4,5/2023</t>
+  </si>
+  <si>
+    <t>4/14-16/2023</t>
   </si>
 </sst>
 </file>
@@ -2302,7 +2308,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A8:K133" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A8:K134" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
   <tableColumns count="11">
     <tableColumn id="1" name="PERIOD" dataDxfId="10"/>
     <tableColumn id="2" name="PARTICULARS" dataDxfId="9"/>
@@ -2649,12 +2655,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:K133"/>
+  <dimension ref="A2:K134"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3690" topLeftCell="A55" activePane="bottomLeft"/>
+      <pane ySplit="3690" topLeftCell="A52" activePane="bottomLeft"/>
       <selection activeCell="F4" sqref="F4:G4"/>
-      <selection pane="bottomLeft" activeCell="B63" sqref="B63"/>
+      <selection pane="bottomLeft" activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2817,7 +2823,7 @@
       <c r="D9" s="11"/>
       <c r="E9" s="13">
         <f>SUM(Table1[EARNED])-SUM(Table1[Absence Undertime W/ Pay])+CONVERTION!$A$3</f>
-        <v>41.25</v>
+        <v>37.5</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="13" t="str">
@@ -2827,7 +2833,7 @@
       <c r="H9" s="11"/>
       <c r="I9" s="13">
         <f>SUM(Table1[[EARNED ]])-SUM(Table1[Absence Undertime  W/ Pay])+CONVERTION!$B$3</f>
-        <v>53.25</v>
+        <v>54.5</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
@@ -3906,13 +3912,15 @@
       <c r="B62" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C62" s="13"/>
+      <c r="C62" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D62" s="39"/>
       <c r="E62" s="9"/>
       <c r="F62" s="20"/>
-      <c r="G62" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G62" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H62" s="39">
         <v>1</v>
@@ -3924,12 +3932,14 @@
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A63" s="40">
-        <v>45047</v>
-      </c>
-      <c r="B63" s="20"/>
+      <c r="A63" s="40"/>
+      <c r="B63" s="20" t="s">
+        <v>54</v>
+      </c>
       <c r="C63" s="13"/>
-      <c r="D63" s="39"/>
+      <c r="D63" s="39">
+        <v>2</v>
+      </c>
       <c r="E63" s="9"/>
       <c r="F63" s="20"/>
       <c r="G63" s="13" t="str">
@@ -3939,15 +3949,21 @@
       <c r="H63" s="39"/>
       <c r="I63" s="9"/>
       <c r="J63" s="11"/>
-      <c r="K63" s="20"/>
+      <c r="K63" s="49" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="40">
-        <v>45078</v>
-      </c>
-      <c r="B64" s="20"/>
+        <v>45047</v>
+      </c>
+      <c r="B64" s="20" t="s">
+        <v>51</v>
+      </c>
       <c r="C64" s="13"/>
-      <c r="D64" s="39"/>
+      <c r="D64" s="39">
+        <v>3</v>
+      </c>
       <c r="E64" s="9"/>
       <c r="F64" s="20"/>
       <c r="G64" s="13" t="str">
@@ -3957,11 +3973,13 @@
       <c r="H64" s="39"/>
       <c r="I64" s="9"/>
       <c r="J64" s="11"/>
-      <c r="K64" s="20"/>
+      <c r="K64" s="20" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="40">
-        <v>45108</v>
+        <v>45078</v>
       </c>
       <c r="B65" s="20"/>
       <c r="C65" s="13"/>
@@ -3979,7 +3997,7 @@
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="40">
-        <v>45139</v>
+        <v>45108</v>
       </c>
       <c r="B66" s="20"/>
       <c r="C66" s="13"/>
@@ -3997,7 +4015,7 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="40">
-        <v>45170</v>
+        <v>45139</v>
       </c>
       <c r="B67" s="20"/>
       <c r="C67" s="13"/>
@@ -4015,7 +4033,7 @@
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="40">
-        <v>45200</v>
+        <v>45170</v>
       </c>
       <c r="B68" s="20"/>
       <c r="C68" s="13"/>
@@ -4033,7 +4051,7 @@
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="40">
-        <v>45231</v>
+        <v>45200</v>
       </c>
       <c r="B69" s="20"/>
       <c r="C69" s="13"/>
@@ -4051,7 +4069,7 @@
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="40">
-        <v>45261</v>
+        <v>45231</v>
       </c>
       <c r="B70" s="20"/>
       <c r="C70" s="13"/>
@@ -4069,7 +4087,7 @@
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="40">
-        <v>45292</v>
+        <v>45261</v>
       </c>
       <c r="B71" s="20"/>
       <c r="C71" s="13"/>
@@ -4087,7 +4105,7 @@
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="40">
-        <v>45323</v>
+        <v>45292</v>
       </c>
       <c r="B72" s="20"/>
       <c r="C72" s="13"/>
@@ -4105,7 +4123,7 @@
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="40">
-        <v>45352</v>
+        <v>45323</v>
       </c>
       <c r="B73" s="20"/>
       <c r="C73" s="13"/>
@@ -4123,7 +4141,7 @@
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="40">
-        <v>45383</v>
+        <v>45352</v>
       </c>
       <c r="B74" s="20"/>
       <c r="C74" s="13"/>
@@ -4141,7 +4159,7 @@
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="40">
-        <v>45413</v>
+        <v>45383</v>
       </c>
       <c r="B75" s="20"/>
       <c r="C75" s="13"/>
@@ -4159,7 +4177,7 @@
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="40">
-        <v>45444</v>
+        <v>45413</v>
       </c>
       <c r="B76" s="20"/>
       <c r="C76" s="13"/>
@@ -4177,7 +4195,7 @@
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="40">
-        <v>45474</v>
+        <v>45444</v>
       </c>
       <c r="B77" s="20"/>
       <c r="C77" s="13"/>
@@ -4195,7 +4213,7 @@
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="40">
-        <v>45505</v>
+        <v>45474</v>
       </c>
       <c r="B78" s="20"/>
       <c r="C78" s="13"/>
@@ -4213,7 +4231,7 @@
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="40">
-        <v>45536</v>
+        <v>45505</v>
       </c>
       <c r="B79" s="20"/>
       <c r="C79" s="13"/>
@@ -4231,7 +4249,7 @@
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="40">
-        <v>45566</v>
+        <v>45536</v>
       </c>
       <c r="B80" s="20"/>
       <c r="C80" s="13"/>
@@ -4249,7 +4267,7 @@
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="40">
-        <v>45597</v>
+        <v>45566</v>
       </c>
       <c r="B81" s="20"/>
       <c r="C81" s="13"/>
@@ -4267,7 +4285,7 @@
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="40">
-        <v>45627</v>
+        <v>45597</v>
       </c>
       <c r="B82" s="20"/>
       <c r="C82" s="13"/>
@@ -4285,7 +4303,7 @@
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="40">
-        <v>45658</v>
+        <v>45627</v>
       </c>
       <c r="B83" s="20"/>
       <c r="C83" s="13"/>
@@ -4303,7 +4321,7 @@
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="40">
-        <v>45689</v>
+        <v>45658</v>
       </c>
       <c r="B84" s="20"/>
       <c r="C84" s="13"/>
@@ -4321,7 +4339,7 @@
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="40">
-        <v>45717</v>
+        <v>45689</v>
       </c>
       <c r="B85" s="20"/>
       <c r="C85" s="13"/>
@@ -4339,7 +4357,7 @@
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="40">
-        <v>45748</v>
+        <v>45717</v>
       </c>
       <c r="B86" s="20"/>
       <c r="C86" s="13"/>
@@ -4357,7 +4375,7 @@
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="40">
-        <v>45778</v>
+        <v>45748</v>
       </c>
       <c r="B87" s="20"/>
       <c r="C87" s="13"/>
@@ -4375,7 +4393,7 @@
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="40">
-        <v>45809</v>
+        <v>45778</v>
       </c>
       <c r="B88" s="20"/>
       <c r="C88" s="13"/>
@@ -4393,7 +4411,7 @@
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="40">
-        <v>45839</v>
+        <v>45809</v>
       </c>
       <c r="B89" s="20"/>
       <c r="C89" s="13"/>
@@ -4411,7 +4429,7 @@
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="40">
-        <v>45870</v>
+        <v>45839</v>
       </c>
       <c r="B90" s="20"/>
       <c r="C90" s="13"/>
@@ -4429,7 +4447,7 @@
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="40">
-        <v>45901</v>
+        <v>45870</v>
       </c>
       <c r="B91" s="20"/>
       <c r="C91" s="13"/>
@@ -4447,7 +4465,7 @@
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="40">
-        <v>45931</v>
+        <v>45901</v>
       </c>
       <c r="B92" s="20"/>
       <c r="C92" s="13"/>
@@ -4465,7 +4483,7 @@
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="40">
-        <v>45962</v>
+        <v>45931</v>
       </c>
       <c r="B93" s="20"/>
       <c r="C93" s="13"/>
@@ -4483,7 +4501,7 @@
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="40">
-        <v>45992</v>
+        <v>45962</v>
       </c>
       <c r="B94" s="20"/>
       <c r="C94" s="13"/>
@@ -4501,7 +4519,7 @@
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="40">
-        <v>46023</v>
+        <v>45992</v>
       </c>
       <c r="B95" s="20"/>
       <c r="C95" s="13"/>
@@ -4519,7 +4537,7 @@
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="40">
-        <v>46054</v>
+        <v>46023</v>
       </c>
       <c r="B96" s="20"/>
       <c r="C96" s="13"/>
@@ -4537,7 +4555,7 @@
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="40">
-        <v>46082</v>
+        <v>46054</v>
       </c>
       <c r="B97" s="20"/>
       <c r="C97" s="13"/>
@@ -4555,7 +4573,7 @@
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="40">
-        <v>46113</v>
+        <v>46082</v>
       </c>
       <c r="B98" s="20"/>
       <c r="C98" s="13"/>
@@ -4573,7 +4591,7 @@
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="40">
-        <v>46143</v>
+        <v>46113</v>
       </c>
       <c r="B99" s="20"/>
       <c r="C99" s="13"/>
@@ -4591,7 +4609,7 @@
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="40">
-        <v>46174</v>
+        <v>46143</v>
       </c>
       <c r="B100" s="20"/>
       <c r="C100" s="13"/>
@@ -4609,7 +4627,7 @@
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="40">
-        <v>46204</v>
+        <v>46174</v>
       </c>
       <c r="B101" s="20"/>
       <c r="C101" s="13"/>
@@ -4627,7 +4645,7 @@
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="40">
-        <v>46235</v>
+        <v>46204</v>
       </c>
       <c r="B102" s="20"/>
       <c r="C102" s="13"/>
@@ -4645,7 +4663,7 @@
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="40">
-        <v>46266</v>
+        <v>46235</v>
       </c>
       <c r="B103" s="20"/>
       <c r="C103" s="13"/>
@@ -4663,7 +4681,7 @@
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="40">
-        <v>46296</v>
+        <v>46266</v>
       </c>
       <c r="B104" s="20"/>
       <c r="C104" s="13"/>
@@ -4681,7 +4699,7 @@
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="40">
-        <v>46327</v>
+        <v>46296</v>
       </c>
       <c r="B105" s="20"/>
       <c r="C105" s="13"/>
@@ -4699,7 +4717,7 @@
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="40">
-        <v>46357</v>
+        <v>46327</v>
       </c>
       <c r="B106" s="20"/>
       <c r="C106" s="13"/>
@@ -4717,7 +4735,7 @@
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="40">
-        <v>46388</v>
+        <v>46357</v>
       </c>
       <c r="B107" s="20"/>
       <c r="C107" s="13"/>
@@ -4735,7 +4753,7 @@
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="40">
-        <v>46419</v>
+        <v>46388</v>
       </c>
       <c r="B108" s="20"/>
       <c r="C108" s="13"/>
@@ -4753,7 +4771,7 @@
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="40">
-        <v>46447</v>
+        <v>46419</v>
       </c>
       <c r="B109" s="20"/>
       <c r="C109" s="13"/>
@@ -4771,7 +4789,7 @@
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="40">
-        <v>46478</v>
+        <v>46447</v>
       </c>
       <c r="B110" s="20"/>
       <c r="C110" s="13"/>
@@ -4789,7 +4807,7 @@
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="40">
-        <v>46508</v>
+        <v>46478</v>
       </c>
       <c r="B111" s="20"/>
       <c r="C111" s="13"/>
@@ -4806,7 +4824,9 @@
       <c r="K111" s="20"/>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A112" s="40"/>
+      <c r="A112" s="40">
+        <v>46508</v>
+      </c>
       <c r="B112" s="20"/>
       <c r="C112" s="13"/>
       <c r="D112" s="39"/>
@@ -5142,20 +5162,36 @@
       <c r="K132" s="20"/>
     </row>
     <row r="133" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A133" s="41"/>
-      <c r="B133" s="15"/>
-      <c r="C133" s="42"/>
-      <c r="D133" s="43"/>
+      <c r="A133" s="40"/>
+      <c r="B133" s="20"/>
+      <c r="C133" s="13"/>
+      <c r="D133" s="39"/>
       <c r="E133" s="9"/>
-      <c r="F133" s="15"/>
-      <c r="G133" s="42" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
-      </c>
-      <c r="H133" s="43"/>
+      <c r="F133" s="20"/>
+      <c r="G133" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H133" s="39"/>
       <c r="I133" s="9"/>
-      <c r="J133" s="12"/>
-      <c r="K133" s="15"/>
+      <c r="J133" s="11"/>
+      <c r="K133" s="20"/>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A134" s="41"/>
+      <c r="B134" s="15"/>
+      <c r="C134" s="42"/>
+      <c r="D134" s="43"/>
+      <c r="E134" s="9"/>
+      <c r="F134" s="15"/>
+      <c r="G134" s="42" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H134" s="43"/>
+      <c r="I134" s="9"/>
+      <c r="J134" s="12"/>
+      <c r="K134" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="11">

</xml_diff>

<commit_message>
Update Leave Card 6/30/2023 4:57 PM
</commit_message>
<xml_diff>
--- a/ANDAG, ALEX.xlsx
+++ b/ANDAG, ALEX.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\DESKTOP-JHL336T\Users\ASUS\Desktop\LEAVE-CARD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\LEAVE-CARD\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C080F1-21D9-480C-B500-7A26AEEC4D7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INSTRUCTION" sheetId="4" r:id="rId1"/>
@@ -24,7 +25,7 @@
     <definedName name="BALANCE_1">Table1[[#Headers],[BALANCE]]</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">Sheet1!$1:$9</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="62">
   <si>
     <t>PERIOD</t>
   </si>
@@ -218,11 +219,14 @@
   <si>
     <t>5/26,29/2023</t>
   </si>
+  <si>
+    <t>7/6,7/2023</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
@@ -910,7 +914,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -953,7 +957,7 @@
         <xdr:cNvPr id="5" name="TextBox 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1017,7 +1021,7 @@
         <xdr:cNvPr id="4" name="Arrow: Left 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1077,7 +1081,7 @@
         <xdr:cNvPr id="8" name="Oval 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1143,7 +1147,7 @@
         <xdr:cNvPr id="9" name="Arrow: Left-Right 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1206,7 +1210,7 @@
         <xdr:cNvPr id="10" name="TextBox 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1304,7 +1308,7 @@
         <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1363,7 +1367,7 @@
         <xdr:cNvPr id="19" name="TextBox 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1428,7 +1432,7 @@
         <xdr:cNvPr id="20" name="Picture 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1471,7 +1475,7 @@
         <xdr:cNvPr id="21" name="TextBox 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1546,7 +1550,7 @@
         <xdr:cNvPr id="22" name="TextBox 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1732,7 +1736,7 @@
         <xdr:cNvPr id="23" name="Oval 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1798,7 +1802,7 @@
         <xdr:cNvPr id="24" name="Straight Arrow Connector 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1856,7 +1860,7 @@
         <xdr:cNvPr id="26" name="Oval 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1922,7 +1926,7 @@
         <xdr:cNvPr id="27" name="Straight Arrow Connector 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1978,7 +1982,7 @@
         <xdr:cNvPr id="30" name="TextBox 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2053,7 +2057,7 @@
         <xdr:cNvPr id="31" name="Picture 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2096,7 +2100,7 @@
         <xdr:cNvPr id="32" name="Oval 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2162,7 +2166,7 @@
         <xdr:cNvPr id="33" name="Straight Arrow Connector 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2218,7 +2222,7 @@
         <xdr:cNvPr id="34" name="TextBox 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2297,7 +2301,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Sheet1"/>
@@ -2314,25 +2318,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A8:K136" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A8:K137" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
   <tableColumns count="11">
-    <tableColumn id="1" name="PERIOD" dataDxfId="10"/>
-    <tableColumn id="2" name="PARTICULARS" dataDxfId="9"/>
-    <tableColumn id="3" name="EARNED" dataDxfId="8"/>
-    <tableColumn id="4" name="Absence Undertime W/ Pay" dataDxfId="7"/>
-    <tableColumn id="5" name="BALANCE" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="PERIOD" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="PARTICULARS" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="EARNED" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Absence Undertime W/ Pay" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="BALANCE" dataDxfId="6">
       <calculatedColumnFormula>SUM(Table1[EARNED])-SUM(Table1[Absence Undertime W/ Pay])+CONVERTION!$A$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Absence Undertime W/O Pay" dataDxfId="5"/>
-    <tableColumn id="7" name="EARNED " dataDxfId="4">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Absence Undertime W/O Pay" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="EARNED " dataDxfId="4">
       <calculatedColumnFormula>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Absence Undertime  W/ Pay" dataDxfId="3"/>
-    <tableColumn id="9" name="BALANCE " dataDxfId="2">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Absence Undertime  W/ Pay" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="BALANCE " dataDxfId="2">
       <calculatedColumnFormula>SUM(Table1[[EARNED ]])-SUM(Table1[Absence Undertime  W/ Pay])+CONVERTION!$B$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Absence Undertime  W/O Pay" dataDxfId="1"/>
-    <tableColumn id="11" name="REMARKS" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Absence Undertime  W/O Pay" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="REMARKS" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -2639,7 +2643,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -2649,7 +2653,7 @@
       <selection activeCell="Z62" sqref="Z62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2657,34 +2661,34 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:K136"/>
+  <dimension ref="A2:K137"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3690" topLeftCell="A55" activePane="bottomLeft"/>
+      <pane ySplit="3696" topLeftCell="A59" activePane="bottomLeft"/>
       <selection activeCell="F4" sqref="F4:G4"/>
-      <selection pane="bottomLeft" activeCell="D69" sqref="D69"/>
+      <selection pane="bottomLeft" activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="30" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" style="30" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="24.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" style="30" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" style="30" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
         <v>9</v>
       </c>
@@ -2705,7 +2709,7 @@
       <c r="J2" s="52"/>
       <c r="K2" s="53"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
@@ -2725,7 +2729,7 @@
       <c r="J3" s="54"/>
       <c r="K3" s="55"/>
     </row>
-    <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
@@ -2747,7 +2751,7 @@
       <c r="J4" s="52"/>
       <c r="K4" s="53"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="H5" s="27" t="s">
         <v>18</v>
@@ -2755,7 +2759,7 @@
       <c r="I5" s="27"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="8"/>
       <c r="C6" s="31"/>
@@ -2768,7 +2772,7 @@
       <c r="J6" s="8"/>
       <c r="K6" s="19"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
       <c r="C7" s="50" t="s">
@@ -2785,7 +2789,7 @@
       <c r="J7" s="50"/>
       <c r="K7" s="14"/>
     </row>
-    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>0</v>
       </c>
@@ -2820,7 +2824,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="23"/>
       <c r="B9" s="24" t="s">
         <v>23</v>
@@ -2829,7 +2833,7 @@
       <c r="D9" s="11"/>
       <c r="E9" s="13">
         <f>SUM(Table1[EARNED])-SUM(Table1[Absence Undertime W/ Pay])+CONVERTION!$A$3</f>
-        <v>38.75</v>
+        <v>38</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="13" t="str">
@@ -2839,12 +2843,12 @@
       <c r="H9" s="11"/>
       <c r="I9" s="13">
         <f>SUM(Table1[[EARNED ]])-SUM(Table1[Absence Undertime  W/ Pay])+CONVERTION!$B$3</f>
-        <v>53.75</v>
+        <v>55</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="48" t="s">
         <v>45</v>
       </c>
@@ -2866,7 +2870,7 @@
       <c r="J10" s="11"/>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="40">
         <v>43647</v>
       </c>
@@ -2886,7 +2890,7 @@
       <c r="J11" s="11"/>
       <c r="K11" s="20"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="40">
         <f>EDATE(A11,1)</f>
         <v>43678</v>
@@ -2907,7 +2911,7 @@
       <c r="J12" s="11"/>
       <c r="K12" s="20"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="40">
         <f t="shared" ref="A13:A16" si="0">EDATE(A12,1)</f>
         <v>43709</v>
@@ -2928,7 +2932,7 @@
       <c r="J13" s="11"/>
       <c r="K13" s="20"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="40">
         <f t="shared" si="0"/>
         <v>43739</v>
@@ -2949,7 +2953,7 @@
       <c r="J14" s="11"/>
       <c r="K14" s="20"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="40">
         <f t="shared" si="0"/>
         <v>43770</v>
@@ -2970,7 +2974,7 @@
       <c r="J15" s="11"/>
       <c r="K15" s="20"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="40">
         <f t="shared" si="0"/>
         <v>43800</v>
@@ -2991,7 +2995,7 @@
       <c r="J16" s="12"/>
       <c r="K16" s="15"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="48" t="s">
         <v>46</v>
       </c>
@@ -3009,7 +3013,7 @@
       <c r="J17" s="11"/>
       <c r="K17" s="20"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="40">
         <v>43831</v>
       </c>
@@ -3029,7 +3033,7 @@
       <c r="J18" s="11"/>
       <c r="K18" s="20"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="40">
         <v>43862</v>
       </c>
@@ -3049,7 +3053,7 @@
       <c r="J19" s="11"/>
       <c r="K19" s="20"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="40">
         <v>43891</v>
       </c>
@@ -3069,7 +3073,7 @@
       <c r="J20" s="11"/>
       <c r="K20" s="20"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="40">
         <v>43922</v>
       </c>
@@ -3089,7 +3093,7 @@
       <c r="J21" s="11"/>
       <c r="K21" s="20"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="40">
         <v>43952</v>
       </c>
@@ -3109,7 +3113,7 @@
       <c r="J22" s="11"/>
       <c r="K22" s="20"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="40">
         <v>43983</v>
       </c>
@@ -3129,7 +3133,7 @@
       <c r="J23" s="11"/>
       <c r="K23" s="20"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="40">
         <v>44013</v>
       </c>
@@ -3149,7 +3153,7 @@
       <c r="J24" s="11"/>
       <c r="K24" s="20"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="40">
         <v>44044</v>
       </c>
@@ -3169,7 +3173,7 @@
       <c r="J25" s="11"/>
       <c r="K25" s="20"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="40">
         <v>44075</v>
       </c>
@@ -3189,7 +3193,7 @@
       <c r="J26" s="11"/>
       <c r="K26" s="20"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="40">
         <v>44105</v>
       </c>
@@ -3209,7 +3213,7 @@
       <c r="J27" s="11"/>
       <c r="K27" s="20"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="40">
         <v>44136</v>
       </c>
@@ -3229,7 +3233,7 @@
       <c r="J28" s="11"/>
       <c r="K28" s="20"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="40">
         <v>44166</v>
       </c>
@@ -3253,7 +3257,7 @@
       <c r="J29" s="11"/>
       <c r="K29" s="20"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="48" t="s">
         <v>47</v>
       </c>
@@ -3271,7 +3275,7 @@
       <c r="J30" s="11"/>
       <c r="K30" s="20"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="40">
         <v>44197</v>
       </c>
@@ -3291,7 +3295,7 @@
       <c r="J31" s="11"/>
       <c r="K31" s="20"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="40">
         <v>44228</v>
       </c>
@@ -3311,7 +3315,7 @@
       <c r="J32" s="11"/>
       <c r="K32" s="20"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="40">
         <v>44256</v>
       </c>
@@ -3331,7 +3335,7 @@
       <c r="J33" s="11"/>
       <c r="K33" s="20"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="40">
         <v>44287</v>
       </c>
@@ -3351,7 +3355,7 @@
       <c r="J34" s="11"/>
       <c r="K34" s="20"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="40">
         <v>44317</v>
       </c>
@@ -3371,7 +3375,7 @@
       <c r="J35" s="11"/>
       <c r="K35" s="20"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="40">
         <v>44348</v>
       </c>
@@ -3391,7 +3395,7 @@
       <c r="J36" s="11"/>
       <c r="K36" s="20"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="40">
         <v>44378</v>
       </c>
@@ -3411,7 +3415,7 @@
       <c r="J37" s="11"/>
       <c r="K37" s="20"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="40">
         <v>44409</v>
       </c>
@@ -3431,7 +3435,7 @@
       <c r="J38" s="11"/>
       <c r="K38" s="20"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="40">
         <v>44440</v>
       </c>
@@ -3451,7 +3455,7 @@
       <c r="J39" s="11"/>
       <c r="K39" s="20"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="40">
         <v>44470</v>
       </c>
@@ -3471,7 +3475,7 @@
       <c r="J40" s="11"/>
       <c r="K40" s="20"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="40">
         <v>44501</v>
       </c>
@@ -3491,7 +3495,7 @@
       <c r="J41" s="11"/>
       <c r="K41" s="20"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="40">
         <v>44531</v>
       </c>
@@ -3515,7 +3519,7 @@
       <c r="J42" s="11"/>
       <c r="K42" s="20"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="48" t="s">
         <v>49</v>
       </c>
@@ -3533,7 +3537,7 @@
       <c r="J43" s="11"/>
       <c r="K43" s="20"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="40">
         <v>44562</v>
       </c>
@@ -3553,7 +3557,7 @@
       <c r="J44" s="11"/>
       <c r="K44" s="20"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="40">
         <v>44593</v>
       </c>
@@ -3573,7 +3577,7 @@
       <c r="J45" s="11"/>
       <c r="K45" s="20"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="40">
         <v>44621</v>
       </c>
@@ -3593,7 +3597,7 @@
       <c r="J46" s="11"/>
       <c r="K46" s="20"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="40">
         <v>44652</v>
       </c>
@@ -3613,7 +3617,7 @@
       <c r="J47" s="11"/>
       <c r="K47" s="20"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="40">
         <v>44682</v>
       </c>
@@ -3639,7 +3643,7 @@
         <v>44687</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="40">
         <v>44713</v>
       </c>
@@ -3659,7 +3663,7 @@
       <c r="J49" s="11"/>
       <c r="K49" s="20"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="40">
         <v>44743</v>
       </c>
@@ -3679,7 +3683,7 @@
       <c r="J50" s="11"/>
       <c r="K50" s="20"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="40">
         <v>44774</v>
       </c>
@@ -3699,7 +3703,7 @@
       <c r="J51" s="11"/>
       <c r="K51" s="20"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="40">
         <v>44805</v>
       </c>
@@ -3719,7 +3723,7 @@
       <c r="J52" s="11"/>
       <c r="K52" s="20"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="40">
         <v>44835</v>
       </c>
@@ -3739,7 +3743,7 @@
       <c r="J53" s="11"/>
       <c r="K53" s="20"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="40">
         <v>44866</v>
       </c>
@@ -3765,7 +3769,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" s="40"/>
       <c r="B55" s="20" t="s">
         <v>54</v>
@@ -3787,7 +3791,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="40"/>
       <c r="B56" s="20" t="s">
         <v>56</v>
@@ -3807,7 +3811,7 @@
         <v>44893</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" s="40">
         <v>44896</v>
       </c>
@@ -3827,7 +3831,7 @@
       <c r="J57" s="11"/>
       <c r="K57" s="20"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" s="48" t="s">
         <v>53</v>
       </c>
@@ -3845,7 +3849,7 @@
       <c r="J58" s="11"/>
       <c r="K58" s="20"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="40">
         <v>44927</v>
       </c>
@@ -3865,7 +3869,7 @@
       <c r="J59" s="11"/>
       <c r="K59" s="20"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="40">
         <v>44958</v>
       </c>
@@ -3891,7 +3895,7 @@
         <v>44962</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="40">
         <v>44986</v>
       </c>
@@ -3911,7 +3915,7 @@
       <c r="J61" s="11"/>
       <c r="K61" s="20"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" s="40">
         <v>45017</v>
       </c>
@@ -3937,7 +3941,7 @@
         <v>45037</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" s="40"/>
       <c r="B63" s="20" t="s">
         <v>54</v>
@@ -3959,7 +3963,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" s="40">
         <v>45047</v>
       </c>
@@ -3985,7 +3989,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="40"/>
       <c r="B65" s="20" t="s">
         <v>59</v>
@@ -4005,20 +4009,22 @@
         <v>60</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="40">
         <v>45078</v>
       </c>
       <c r="B66" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C66" s="13"/>
+      <c r="C66" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D66" s="39"/>
       <c r="E66" s="9"/>
       <c r="F66" s="20"/>
-      <c r="G66" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G66" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H66" s="39">
         <v>1</v>
@@ -4029,7 +4035,7 @@
         <v>45081</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" s="40"/>
       <c r="B67" s="20" t="s">
         <v>50</v>
@@ -4051,13 +4057,15 @@
         <v>45085</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A68" s="40">
-        <v>45108</v>
-      </c>
-      <c r="B68" s="20"/>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A68" s="40"/>
+      <c r="B68" s="20" t="s">
+        <v>54</v>
+      </c>
       <c r="C68" s="13"/>
-      <c r="D68" s="39"/>
+      <c r="D68" s="39">
+        <v>2</v>
+      </c>
       <c r="E68" s="9"/>
       <c r="F68" s="20"/>
       <c r="G68" s="13" t="str">
@@ -4067,11 +4075,13 @@
       <c r="H68" s="39"/>
       <c r="I68" s="9"/>
       <c r="J68" s="11"/>
-      <c r="K68" s="20"/>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K68" s="49" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" s="40">
-        <v>45139</v>
+        <v>45108</v>
       </c>
       <c r="B69" s="20"/>
       <c r="C69" s="13"/>
@@ -4087,9 +4097,9 @@
       <c r="J69" s="11"/>
       <c r="K69" s="20"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" s="40">
-        <v>45170</v>
+        <v>45139</v>
       </c>
       <c r="B70" s="20"/>
       <c r="C70" s="13"/>
@@ -4105,9 +4115,9 @@
       <c r="J70" s="11"/>
       <c r="K70" s="20"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" s="40">
-        <v>45200</v>
+        <v>45170</v>
       </c>
       <c r="B71" s="20"/>
       <c r="C71" s="13"/>
@@ -4123,9 +4133,9 @@
       <c r="J71" s="11"/>
       <c r="K71" s="20"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" s="40">
-        <v>45231</v>
+        <v>45200</v>
       </c>
       <c r="B72" s="20"/>
       <c r="C72" s="13"/>
@@ -4141,9 +4151,9 @@
       <c r="J72" s="11"/>
       <c r="K72" s="20"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" s="40">
-        <v>45261</v>
+        <v>45231</v>
       </c>
       <c r="B73" s="20"/>
       <c r="C73" s="13"/>
@@ -4159,9 +4169,9 @@
       <c r="J73" s="11"/>
       <c r="K73" s="20"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" s="40">
-        <v>45292</v>
+        <v>45261</v>
       </c>
       <c r="B74" s="20"/>
       <c r="C74" s="13"/>
@@ -4177,9 +4187,9 @@
       <c r="J74" s="11"/>
       <c r="K74" s="20"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" s="40">
-        <v>45323</v>
+        <v>45292</v>
       </c>
       <c r="B75" s="20"/>
       <c r="C75" s="13"/>
@@ -4195,9 +4205,9 @@
       <c r="J75" s="11"/>
       <c r="K75" s="20"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" s="40">
-        <v>45352</v>
+        <v>45323</v>
       </c>
       <c r="B76" s="20"/>
       <c r="C76" s="13"/>
@@ -4213,9 +4223,9 @@
       <c r="J76" s="11"/>
       <c r="K76" s="20"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" s="40">
-        <v>45383</v>
+        <v>45352</v>
       </c>
       <c r="B77" s="20"/>
       <c r="C77" s="13"/>
@@ -4231,9 +4241,9 @@
       <c r="J77" s="11"/>
       <c r="K77" s="20"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" s="40">
-        <v>45413</v>
+        <v>45383</v>
       </c>
       <c r="B78" s="20"/>
       <c r="C78" s="13"/>
@@ -4249,9 +4259,9 @@
       <c r="J78" s="11"/>
       <c r="K78" s="20"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" s="40">
-        <v>45444</v>
+        <v>45413</v>
       </c>
       <c r="B79" s="20"/>
       <c r="C79" s="13"/>
@@ -4267,9 +4277,9 @@
       <c r="J79" s="11"/>
       <c r="K79" s="20"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" s="40">
-        <v>45474</v>
+        <v>45444</v>
       </c>
       <c r="B80" s="20"/>
       <c r="C80" s="13"/>
@@ -4285,9 +4295,9 @@
       <c r="J80" s="11"/>
       <c r="K80" s="20"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" s="40">
-        <v>45505</v>
+        <v>45474</v>
       </c>
       <c r="B81" s="20"/>
       <c r="C81" s="13"/>
@@ -4303,9 +4313,9 @@
       <c r="J81" s="11"/>
       <c r="K81" s="20"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" s="40">
-        <v>45536</v>
+        <v>45505</v>
       </c>
       <c r="B82" s="20"/>
       <c r="C82" s="13"/>
@@ -4321,9 +4331,9 @@
       <c r="J82" s="11"/>
       <c r="K82" s="20"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" s="40">
-        <v>45566</v>
+        <v>45536</v>
       </c>
       <c r="B83" s="20"/>
       <c r="C83" s="13"/>
@@ -4339,9 +4349,9 @@
       <c r="J83" s="11"/>
       <c r="K83" s="20"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" s="40">
-        <v>45597</v>
+        <v>45566</v>
       </c>
       <c r="B84" s="20"/>
       <c r="C84" s="13"/>
@@ -4357,9 +4367,9 @@
       <c r="J84" s="11"/>
       <c r="K84" s="20"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85" s="40">
-        <v>45627</v>
+        <v>45597</v>
       </c>
       <c r="B85" s="20"/>
       <c r="C85" s="13"/>
@@ -4375,9 +4385,9 @@
       <c r="J85" s="11"/>
       <c r="K85" s="20"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86" s="40">
-        <v>45658</v>
+        <v>45627</v>
       </c>
       <c r="B86" s="20"/>
       <c r="C86" s="13"/>
@@ -4393,9 +4403,9 @@
       <c r="J86" s="11"/>
       <c r="K86" s="20"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87" s="40">
-        <v>45689</v>
+        <v>45658</v>
       </c>
       <c r="B87" s="20"/>
       <c r="C87" s="13"/>
@@ -4411,9 +4421,9 @@
       <c r="J87" s="11"/>
       <c r="K87" s="20"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88" s="40">
-        <v>45717</v>
+        <v>45689</v>
       </c>
       <c r="B88" s="20"/>
       <c r="C88" s="13"/>
@@ -4429,9 +4439,9 @@
       <c r="J88" s="11"/>
       <c r="K88" s="20"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89" s="40">
-        <v>45748</v>
+        <v>45717</v>
       </c>
       <c r="B89" s="20"/>
       <c r="C89" s="13"/>
@@ -4447,9 +4457,9 @@
       <c r="J89" s="11"/>
       <c r="K89" s="20"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90" s="40">
-        <v>45778</v>
+        <v>45748</v>
       </c>
       <c r="B90" s="20"/>
       <c r="C90" s="13"/>
@@ -4465,9 +4475,9 @@
       <c r="J90" s="11"/>
       <c r="K90" s="20"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91" s="40">
-        <v>45809</v>
+        <v>45778</v>
       </c>
       <c r="B91" s="20"/>
       <c r="C91" s="13"/>
@@ -4483,9 +4493,9 @@
       <c r="J91" s="11"/>
       <c r="K91" s="20"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92" s="40">
-        <v>45839</v>
+        <v>45809</v>
       </c>
       <c r="B92" s="20"/>
       <c r="C92" s="13"/>
@@ -4501,9 +4511,9 @@
       <c r="J92" s="11"/>
       <c r="K92" s="20"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93" s="40">
-        <v>45870</v>
+        <v>45839</v>
       </c>
       <c r="B93" s="20"/>
       <c r="C93" s="13"/>
@@ -4519,9 +4529,9 @@
       <c r="J93" s="11"/>
       <c r="K93" s="20"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94" s="40">
-        <v>45901</v>
+        <v>45870</v>
       </c>
       <c r="B94" s="20"/>
       <c r="C94" s="13"/>
@@ -4537,9 +4547,9 @@
       <c r="J94" s="11"/>
       <c r="K94" s="20"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A95" s="40">
-        <v>45931</v>
+        <v>45901</v>
       </c>
       <c r="B95" s="20"/>
       <c r="C95" s="13"/>
@@ -4555,9 +4565,9 @@
       <c r="J95" s="11"/>
       <c r="K95" s="20"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A96" s="40">
-        <v>45962</v>
+        <v>45931</v>
       </c>
       <c r="B96" s="20"/>
       <c r="C96" s="13"/>
@@ -4573,9 +4583,9 @@
       <c r="J96" s="11"/>
       <c r="K96" s="20"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A97" s="40">
-        <v>45992</v>
+        <v>45962</v>
       </c>
       <c r="B97" s="20"/>
       <c r="C97" s="13"/>
@@ -4591,9 +4601,9 @@
       <c r="J97" s="11"/>
       <c r="K97" s="20"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A98" s="40">
-        <v>46023</v>
+        <v>45992</v>
       </c>
       <c r="B98" s="20"/>
       <c r="C98" s="13"/>
@@ -4609,9 +4619,9 @@
       <c r="J98" s="11"/>
       <c r="K98" s="20"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A99" s="40">
-        <v>46054</v>
+        <v>46023</v>
       </c>
       <c r="B99" s="20"/>
       <c r="C99" s="13"/>
@@ -4627,9 +4637,9 @@
       <c r="J99" s="11"/>
       <c r="K99" s="20"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A100" s="40">
-        <v>46082</v>
+        <v>46054</v>
       </c>
       <c r="B100" s="20"/>
       <c r="C100" s="13"/>
@@ -4645,9 +4655,9 @@
       <c r="J100" s="11"/>
       <c r="K100" s="20"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A101" s="40">
-        <v>46113</v>
+        <v>46082</v>
       </c>
       <c r="B101" s="20"/>
       <c r="C101" s="13"/>
@@ -4663,9 +4673,9 @@
       <c r="J101" s="11"/>
       <c r="K101" s="20"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A102" s="40">
-        <v>46143</v>
+        <v>46113</v>
       </c>
       <c r="B102" s="20"/>
       <c r="C102" s="13"/>
@@ -4681,9 +4691,9 @@
       <c r="J102" s="11"/>
       <c r="K102" s="20"/>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A103" s="40">
-        <v>46174</v>
+        <v>46143</v>
       </c>
       <c r="B103" s="20"/>
       <c r="C103" s="13"/>
@@ -4699,9 +4709,9 @@
       <c r="J103" s="11"/>
       <c r="K103" s="20"/>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A104" s="40">
-        <v>46204</v>
+        <v>46174</v>
       </c>
       <c r="B104" s="20"/>
       <c r="C104" s="13"/>
@@ -4717,9 +4727,9 @@
       <c r="J104" s="11"/>
       <c r="K104" s="20"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A105" s="40">
-        <v>46235</v>
+        <v>46204</v>
       </c>
       <c r="B105" s="20"/>
       <c r="C105" s="13"/>
@@ -4735,9 +4745,9 @@
       <c r="J105" s="11"/>
       <c r="K105" s="20"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A106" s="40">
-        <v>46266</v>
+        <v>46235</v>
       </c>
       <c r="B106" s="20"/>
       <c r="C106" s="13"/>
@@ -4753,9 +4763,9 @@
       <c r="J106" s="11"/>
       <c r="K106" s="20"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A107" s="40">
-        <v>46296</v>
+        <v>46266</v>
       </c>
       <c r="B107" s="20"/>
       <c r="C107" s="13"/>
@@ -4771,9 +4781,9 @@
       <c r="J107" s="11"/>
       <c r="K107" s="20"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A108" s="40">
-        <v>46327</v>
+        <v>46296</v>
       </c>
       <c r="B108" s="20"/>
       <c r="C108" s="13"/>
@@ -4789,9 +4799,9 @@
       <c r="J108" s="11"/>
       <c r="K108" s="20"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A109" s="40">
-        <v>46357</v>
+        <v>46327</v>
       </c>
       <c r="B109" s="20"/>
       <c r="C109" s="13"/>
@@ -4807,9 +4817,9 @@
       <c r="J109" s="11"/>
       <c r="K109" s="20"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A110" s="40">
-        <v>46388</v>
+        <v>46357</v>
       </c>
       <c r="B110" s="20"/>
       <c r="C110" s="13"/>
@@ -4825,9 +4835,9 @@
       <c r="J110" s="11"/>
       <c r="K110" s="20"/>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A111" s="40">
-        <v>46419</v>
+        <v>46388</v>
       </c>
       <c r="B111" s="20"/>
       <c r="C111" s="13"/>
@@ -4843,9 +4853,9 @@
       <c r="J111" s="11"/>
       <c r="K111" s="20"/>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A112" s="40">
-        <v>46447</v>
+        <v>46419</v>
       </c>
       <c r="B112" s="20"/>
       <c r="C112" s="13"/>
@@ -4861,9 +4871,9 @@
       <c r="J112" s="11"/>
       <c r="K112" s="20"/>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A113" s="40">
-        <v>46478</v>
+        <v>46447</v>
       </c>
       <c r="B113" s="20"/>
       <c r="C113" s="13"/>
@@ -4879,9 +4889,9 @@
       <c r="J113" s="11"/>
       <c r="K113" s="20"/>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A114" s="40">
-        <v>46508</v>
+        <v>46478</v>
       </c>
       <c r="B114" s="20"/>
       <c r="C114" s="13"/>
@@ -4897,8 +4907,10 @@
       <c r="J114" s="11"/>
       <c r="K114" s="20"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A115" s="40"/>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A115" s="40">
+        <v>46508</v>
+      </c>
       <c r="B115" s="20"/>
       <c r="C115" s="13"/>
       <c r="D115" s="39"/>
@@ -4913,7 +4925,7 @@
       <c r="J115" s="11"/>
       <c r="K115" s="20"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A116" s="40"/>
       <c r="B116" s="20"/>
       <c r="C116" s="13"/>
@@ -4929,7 +4941,7 @@
       <c r="J116" s="11"/>
       <c r="K116" s="20"/>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A117" s="40"/>
       <c r="B117" s="20"/>
       <c r="C117" s="13"/>
@@ -4945,7 +4957,7 @@
       <c r="J117" s="11"/>
       <c r="K117" s="20"/>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A118" s="40"/>
       <c r="B118" s="20"/>
       <c r="C118" s="13"/>
@@ -4961,7 +4973,7 @@
       <c r="J118" s="11"/>
       <c r="K118" s="20"/>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A119" s="40"/>
       <c r="B119" s="20"/>
       <c r="C119" s="13"/>
@@ -4977,7 +4989,7 @@
       <c r="J119" s="11"/>
       <c r="K119" s="20"/>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A120" s="40"/>
       <c r="B120" s="20"/>
       <c r="C120" s="13"/>
@@ -4993,7 +5005,7 @@
       <c r="J120" s="11"/>
       <c r="K120" s="20"/>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A121" s="40"/>
       <c r="B121" s="20"/>
       <c r="C121" s="13"/>
@@ -5009,7 +5021,7 @@
       <c r="J121" s="11"/>
       <c r="K121" s="20"/>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A122" s="40"/>
       <c r="B122" s="20"/>
       <c r="C122" s="13"/>
@@ -5025,7 +5037,7 @@
       <c r="J122" s="11"/>
       <c r="K122" s="20"/>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A123" s="40"/>
       <c r="B123" s="20"/>
       <c r="C123" s="13"/>
@@ -5041,7 +5053,7 @@
       <c r="J123" s="11"/>
       <c r="K123" s="20"/>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A124" s="40"/>
       <c r="B124" s="20"/>
       <c r="C124" s="13"/>
@@ -5057,7 +5069,7 @@
       <c r="J124" s="11"/>
       <c r="K124" s="20"/>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A125" s="40"/>
       <c r="B125" s="20"/>
       <c r="C125" s="13"/>
@@ -5073,7 +5085,7 @@
       <c r="J125" s="11"/>
       <c r="K125" s="20"/>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A126" s="40"/>
       <c r="B126" s="20"/>
       <c r="C126" s="13"/>
@@ -5089,7 +5101,7 @@
       <c r="J126" s="11"/>
       <c r="K126" s="20"/>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A127" s="40"/>
       <c r="B127" s="20"/>
       <c r="C127" s="13"/>
@@ -5105,7 +5117,7 @@
       <c r="J127" s="11"/>
       <c r="K127" s="20"/>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A128" s="40"/>
       <c r="B128" s="20"/>
       <c r="C128" s="13"/>
@@ -5121,7 +5133,7 @@
       <c r="J128" s="11"/>
       <c r="K128" s="20"/>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A129" s="40"/>
       <c r="B129" s="20"/>
       <c r="C129" s="13"/>
@@ -5137,7 +5149,7 @@
       <c r="J129" s="11"/>
       <c r="K129" s="20"/>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A130" s="40"/>
       <c r="B130" s="20"/>
       <c r="C130" s="13"/>
@@ -5153,7 +5165,7 @@
       <c r="J130" s="11"/>
       <c r="K130" s="20"/>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A131" s="40"/>
       <c r="B131" s="20"/>
       <c r="C131" s="13"/>
@@ -5169,7 +5181,7 @@
       <c r="J131" s="11"/>
       <c r="K131" s="20"/>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A132" s="40"/>
       <c r="B132" s="20"/>
       <c r="C132" s="13"/>
@@ -5185,7 +5197,7 @@
       <c r="J132" s="11"/>
       <c r="K132" s="20"/>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A133" s="40"/>
       <c r="B133" s="20"/>
       <c r="C133" s="13"/>
@@ -5201,7 +5213,7 @@
       <c r="J133" s="11"/>
       <c r="K133" s="20"/>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A134" s="40"/>
       <c r="B134" s="20"/>
       <c r="C134" s="13"/>
@@ -5217,7 +5229,7 @@
       <c r="J134" s="11"/>
       <c r="K134" s="20"/>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A135" s="40"/>
       <c r="B135" s="20"/>
       <c r="C135" s="13"/>
@@ -5233,21 +5245,37 @@
       <c r="J135" s="11"/>
       <c r="K135" s="20"/>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A136" s="41"/>
-      <c r="B136" s="15"/>
-      <c r="C136" s="42"/>
-      <c r="D136" s="43"/>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A136" s="40"/>
+      <c r="B136" s="20"/>
+      <c r="C136" s="13"/>
+      <c r="D136" s="39"/>
       <c r="E136" s="9"/>
-      <c r="F136" s="15"/>
-      <c r="G136" s="42" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
-      </c>
-      <c r="H136" s="43"/>
+      <c r="F136" s="20"/>
+      <c r="G136" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H136" s="39"/>
       <c r="I136" s="9"/>
-      <c r="J136" s="12"/>
-      <c r="K136" s="15"/>
+      <c r="J136" s="11"/>
+      <c r="K136" s="20"/>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A137" s="41"/>
+      <c r="B137" s="15"/>
+      <c r="C137" s="42"/>
+      <c r="D137" s="43"/>
+      <c r="E137" s="9"/>
+      <c r="F137" s="15"/>
+      <c r="G137" s="42" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H137" s="43"/>
+      <c r="I137" s="9"/>
+      <c r="J137" s="12"/>
+      <c r="K137" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -5264,10 +5292,10 @@
     <mergeCell ref="F4:G4"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"1 - Married (and not separated), 2 - Widowed (including living common law), 3 - Separated (including living common law), 4 - Divorced (including living common law), 5 - Single (including living common law)"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"PERMANENT, CO-TERMINUS, CASUAL, JOBCON"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5290,28 +5318,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I1" sqref="I1:L1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.140625" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" style="37" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.109375" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.88671875" customWidth="1"/>
+    <col min="11" max="11" width="14.88671875" style="37" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D1" s="58" t="s">
         <v>33</v>
       </c>
@@ -5324,7 +5352,7 @@
       <c r="K1" s="59"/>
       <c r="L1" s="59"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
         <v>24</v>
       </c>
@@ -5353,7 +5381,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="D3" s="11"/>
@@ -5373,17 +5401,17 @@
         <v>---</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="G4" s="33"/>
       <c r="J4" s="1" t="str">
         <f>IF(TEXT(J3,"D")=1,1,TEXT(J3,"D"))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C6" s="38" t="s">
         <v>28</v>
       </c>
@@ -5404,7 +5432,7 @@
       <c r="K6" s="60"/>
       <c r="L6" s="60"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C7" s="37">
         <v>1</v>
       </c>
@@ -5431,7 +5459,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C8" s="37">
         <v>2</v>
       </c>
@@ -5457,7 +5485,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C9" s="37">
         <v>3</v>
       </c>
@@ -5483,7 +5511,7 @@
         <v>8.3000000000000004E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C10" s="37">
         <v>4</v>
       </c>
@@ -5509,7 +5537,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C11" s="37">
         <v>5</v>
       </c>
@@ -5535,7 +5563,7 @@
         <v>0.16700000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C12" s="37">
         <v>6</v>
       </c>
@@ -5561,7 +5589,7 @@
         <v>0.20800000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C13" s="37">
         <v>7</v>
       </c>
@@ -5587,7 +5615,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C14" s="37">
         <v>8</v>
       </c>
@@ -5613,7 +5641,7 @@
         <v>0.29199999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C15" s="37">
         <v>9</v>
       </c>
@@ -5633,7 +5661,7 @@
         <v>0.33299999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C16" s="37">
         <v>10</v>
       </c>
@@ -5653,7 +5681,7 @@
         <v>0.37499999999999994</v>
       </c>
     </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C17" s="37">
         <v>11</v>
       </c>
@@ -5673,7 +5701,7 @@
         <v>0.41699999999999993</v>
       </c>
     </row>
-    <row r="18" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C18" s="37">
         <v>12</v>
       </c>
@@ -5694,7 +5722,7 @@
         <v>0.45799999999999991</v>
       </c>
     </row>
-    <row r="19" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C19" s="37">
         <v>13</v>
       </c>
@@ -5715,7 +5743,7 @@
         <v>0.49999999999999989</v>
       </c>
     </row>
-    <row r="20" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C20" s="37">
         <v>14</v>
       </c>
@@ -5736,7 +5764,7 @@
         <v>0.54199999999999993</v>
       </c>
     </row>
-    <row r="21" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C21" s="37">
         <v>15</v>
       </c>
@@ -5757,7 +5785,7 @@
         <v>0.58299999999999996</v>
       </c>
     </row>
-    <row r="22" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C22" s="37">
         <v>16</v>
       </c>
@@ -5778,7 +5806,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="23" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C23" s="37">
         <v>17</v>
       </c>
@@ -5799,7 +5827,7 @@
         <v>0.66700000000000004</v>
       </c>
     </row>
-    <row r="24" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C24" s="37">
         <v>18</v>
       </c>
@@ -5820,7 +5848,7 @@
         <v>0.70800000000000007</v>
       </c>
     </row>
-    <row r="25" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C25" s="37">
         <v>19</v>
       </c>
@@ -5841,7 +5869,7 @@
         <v>0.75000000000000011</v>
       </c>
     </row>
-    <row r="26" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C26" s="37">
         <v>20</v>
       </c>
@@ -5862,7 +5890,7 @@
         <v>0.79200000000000015</v>
       </c>
     </row>
-    <row r="27" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C27" s="37">
         <v>21</v>
       </c>
@@ -5883,7 +5911,7 @@
         <v>0.83300000000000018</v>
       </c>
     </row>
-    <row r="28" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C28" s="37">
         <v>22</v>
       </c>
@@ -5904,7 +5932,7 @@
         <v>0.87500000000000022</v>
       </c>
     </row>
-    <row r="29" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C29" s="37">
         <v>23</v>
       </c>
@@ -5925,7 +5953,7 @@
         <v>0.91700000000000026</v>
       </c>
     </row>
-    <row r="30" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C30" s="37">
         <v>24</v>
       </c>
@@ -5946,7 +5974,7 @@
         <v>0.9580000000000003</v>
       </c>
     </row>
-    <row r="31" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C31" s="37">
         <v>25</v>
       </c>
@@ -5967,7 +5995,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="32" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C32" s="37">
         <v>26</v>
       </c>
@@ -5988,7 +6016,7 @@
         <v>1.0420000000000003</v>
       </c>
     </row>
-    <row r="33" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C33" s="37">
         <v>27</v>
       </c>
@@ -6009,7 +6037,7 @@
         <v>1.0830000000000002</v>
       </c>
     </row>
-    <row r="34" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C34" s="37">
         <v>28</v>
       </c>
@@ -6030,7 +6058,7 @@
         <v>1.1250000000000002</v>
       </c>
     </row>
-    <row r="35" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C35" s="37">
         <v>29</v>
       </c>
@@ -6051,7 +6079,7 @@
         <v>1.1670000000000003</v>
       </c>
     </row>
-    <row r="36" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C36" s="37">
         <v>30</v>
       </c>
@@ -6072,7 +6100,7 @@
         <v>1.2080000000000002</v>
       </c>
     </row>
-    <row r="37" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C37" s="37">
         <v>31</v>
       </c>
@@ -6093,7 +6121,7 @@
         <v>1.2500000000000002</v>
       </c>
     </row>
-    <row r="38" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C38" s="37">
         <v>32</v>
       </c>
@@ -6102,7 +6130,7 @@
       </c>
       <c r="G38"/>
     </row>
-    <row r="39" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C39" s="37">
         <v>33</v>
       </c>
@@ -6111,7 +6139,7 @@
       </c>
       <c r="G39"/>
     </row>
-    <row r="40" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C40" s="37">
         <v>34</v>
       </c>
@@ -6120,7 +6148,7 @@
       </c>
       <c r="G40"/>
     </row>
-    <row r="41" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C41" s="37">
         <v>35</v>
       </c>
@@ -6129,7 +6157,7 @@
       </c>
       <c r="G41"/>
     </row>
-    <row r="42" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C42" s="37">
         <v>36</v>
       </c>
@@ -6138,7 +6166,7 @@
       </c>
       <c r="G42"/>
     </row>
-    <row r="43" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C43" s="37">
         <v>37</v>
       </c>
@@ -6147,7 +6175,7 @@
       </c>
       <c r="G43"/>
     </row>
-    <row r="44" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C44" s="37">
         <v>38</v>
       </c>
@@ -6156,7 +6184,7 @@
       </c>
       <c r="G44"/>
     </row>
-    <row r="45" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C45" s="37">
         <v>39</v>
       </c>
@@ -6165,7 +6193,7 @@
       </c>
       <c r="G45"/>
     </row>
-    <row r="46" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C46" s="37">
         <v>40</v>
       </c>
@@ -6174,7 +6202,7 @@
       </c>
       <c r="G46"/>
     </row>
-    <row r="47" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C47" s="37">
         <v>41</v>
       </c>
@@ -6183,7 +6211,7 @@
       </c>
       <c r="G47"/>
     </row>
-    <row r="48" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C48" s="37">
         <v>42</v>
       </c>
@@ -6192,7 +6220,7 @@
       </c>
       <c r="G48"/>
     </row>
-    <row r="49" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C49" s="37">
         <v>43</v>
       </c>
@@ -6201,7 +6229,7 @@
       </c>
       <c r="G49"/>
     </row>
-    <row r="50" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C50" s="37">
         <v>44</v>
       </c>
@@ -6210,7 +6238,7 @@
       </c>
       <c r="G50"/>
     </row>
-    <row r="51" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C51" s="37">
         <v>45</v>
       </c>
@@ -6219,7 +6247,7 @@
       </c>
       <c r="G51"/>
     </row>
-    <row r="52" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C52" s="37">
         <v>46</v>
       </c>
@@ -6228,7 +6256,7 @@
       </c>
       <c r="G52"/>
     </row>
-    <row r="53" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C53" s="37">
         <v>47</v>
       </c>
@@ -6237,7 +6265,7 @@
       </c>
       <c r="G53"/>
     </row>
-    <row r="54" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C54" s="37">
         <v>48</v>
       </c>
@@ -6246,7 +6274,7 @@
       </c>
       <c r="G54"/>
     </row>
-    <row r="55" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C55" s="37">
         <v>49</v>
       </c>
@@ -6255,7 +6283,7 @@
       </c>
       <c r="G55"/>
     </row>
-    <row r="56" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C56" s="37">
         <v>50</v>
       </c>
@@ -6264,7 +6292,7 @@
       </c>
       <c r="G56"/>
     </row>
-    <row r="57" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C57" s="37">
         <v>51</v>
       </c>
@@ -6273,7 +6301,7 @@
       </c>
       <c r="G57"/>
     </row>
-    <row r="58" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C58" s="37">
         <v>52</v>
       </c>
@@ -6282,7 +6310,7 @@
       </c>
       <c r="G58"/>
     </row>
-    <row r="59" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C59" s="37">
         <v>53</v>
       </c>
@@ -6291,7 +6319,7 @@
       </c>
       <c r="G59"/>
     </row>
-    <row r="60" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C60" s="37">
         <v>54</v>
       </c>
@@ -6300,7 +6328,7 @@
       </c>
       <c r="G60"/>
     </row>
-    <row r="61" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C61" s="37">
         <v>55</v>
       </c>
@@ -6309,7 +6337,7 @@
       </c>
       <c r="G61"/>
     </row>
-    <row r="62" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C62" s="37">
         <v>56</v>
       </c>
@@ -6318,7 +6346,7 @@
       </c>
       <c r="G62"/>
     </row>
-    <row r="63" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C63" s="37">
         <v>57</v>
       </c>
@@ -6327,7 +6355,7 @@
       </c>
       <c r="G63"/>
     </row>
-    <row r="64" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C64" s="37">
         <v>58</v>
       </c>
@@ -6336,7 +6364,7 @@
       </c>
       <c r="G64"/>
     </row>
-    <row r="65" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C65" s="37">
         <v>59</v>
       </c>
@@ -6345,7 +6373,7 @@
       </c>
       <c r="G65"/>
     </row>
-    <row r="66" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C66" s="37">
         <v>60</v>
       </c>
@@ -6354,7 +6382,7 @@
       </c>
       <c r="G66"/>
     </row>
-    <row r="67" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:12" x14ac:dyDescent="0.3">
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>

</xml_diff>